<commit_message>
Added Capabilities from Arma, CGOC and ISACA_COBIT. Modified query to get all results and more compact.
</commit_message>
<xml_diff>
--- a/excel/IGDSL-MaturityLevelsv0.xlsx
+++ b/excel/IGDSL-MaturityLevelsv0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6DC80D-F870-4F17-A4C3-8543A5E6F388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D26B1A-142A-4101-875F-E420145FB40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="6600" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="87252" yWindow="-108" windowWidth="30936" windowHeight="16284" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GlossariesComparison" sheetId="25" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="1035">
   <si>
     <t>The Enterprise</t>
   </si>
@@ -5828,6 +5828,98 @@
 Der Data Controller ist primär für die Verwaltung, Kontrolle und Einhaltung von Datenschutzbestimmungen und -richtlinien verantwortlich. Die Wahrung der Authentizität von Informationen fällt unter die Verantwortung des Data Controllers, da dies eng mit der Verarbeitung und dem Schutz personenbezogener Daten verbunden ist.
 Der  CSO ist für die Sicherheit von Informationen und Daten in der Organisation verantwortlich. Die Sicherheit von Metadaten, insbesondere im Hinblick auf die Authentizität, ist ein wichtiger Aspekt des Informationssicherheitsmanagements, den der CSO überwacht und sicherstellt.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization consistently defines strategic IT plans that align with business objectives and takes steps to review and adjust these plans periodically.
+ </t>
+  </si>
+  <si>
+    <t>The organization establishes a formalized process for developing and maintaining strategic IT plans. These plans are documented, shared, and aligned with overall business strategies.</t>
+  </si>
+  <si>
+    <t>The organization continuously monitors and improves its strategic IT planning process. It actively seeks feedback from stakeholders, adapts plans to changing circumstances, and demonstrates the agility to respond to emerging technologies and market shifts.</t>
+  </si>
+  <si>
+    <t>The organization ensures that information architecture is defined and consistently applied to technology solutions. Periodic reviews occur to assess alignment with business needs.</t>
+  </si>
+  <si>
+    <t>The organization establishes a comprehensive framework for information architecture design and implementation. There is a structured approach for capturing and managing metadata, data standards, and information flows.</t>
+  </si>
+  <si>
+    <t>The organization continuously evolves its information architecture to accommodate changing business requirements and emerging technologies. Collaboration with stakeholders ensures that information assets are well-structured, accessible, and support innovation.</t>
+  </si>
+  <si>
+    <t>The organization consistently evaluates emerging technologies and assesses their potential alignment with business needs. Decisions are documented, and regular reviews ensure relevance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The organization establishes a structured process for evaluating, selecting, and adopting new technologies. Decision-making criteria, risk assessments, and integration strategies are documented and communicated.</t>
+  </si>
+  <si>
+    <t>The organization actively monitors the technology landscape, anticipates industry trends, and proactively experiments with innovative technologies. Continuous improvement of the technological direction process supports business agility and competitive advantage.</t>
+  </si>
+  <si>
+    <t>The organization consistently defines and documents IT processes, organizational structures, and relationships with stakeholders. Periodic reviews ensure that these components remain aligned with business goals.</t>
+  </si>
+  <si>
+    <t>The organization establishes a well-structured framework for defining, documenting, and communicating IT processes, roles, and responsibilities. Clear relationships and dependencies with other business units are documented and managed.</t>
+  </si>
+  <si>
+    <t>The organization continually assesses the effectiveness of its IT processes, organization, and relationships. Feedback loops and cross-functional collaboration lead to refinements that enhance agility, alignment, and value delivery.</t>
+  </si>
+  <si>
+    <t>The organization consistently manages IT investments through budgeting and tracking financial performance. Regular reviews ensure alignment with business priorities.</t>
+  </si>
+  <si>
+    <t>The organization establishes a structured process for evaluating, prioritizing, and funding IT initiatives. Financial performance is monitored and reported against planned outcomes.</t>
+  </si>
+  <si>
+    <t>The organization actively optimizes its IT investment management process. It demonstrates the ability to dynamically reallocate resources based on changing business needs, risk profiles, and value potential.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The organization consistently communicates management aims and IT directions to relevant stakeholders. Feedback mechanisms exist to gauge alignment and effectiveness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The organization establishes a structured communication plan for conveying management aims and IT directions. Multiple channels are used to ensure clear, consistent, and timely communication.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The organization actively seeks feedback on the effectiveness of communication efforts. Continuous improvement initiatives refine communication strategies to maximize stakeholder understanding and engagement.</t>
+  </si>
+  <si>
+    <t>The organization consistently manages IT human resources through recruitment, training, and performance reviews. Basic workforce planning is in place.</t>
+  </si>
+  <si>
+    <t>The organization establishes a comprehensive human resource management framework for IT. There are structured processes for recruitment, skills development, career progression, and succession planning.</t>
+  </si>
+  <si>
+    <t>The organization actively anticipates future IT workforce needs and adapts human resource strategies accordingly. Continuous learning, talent retention, and effective collaboration contribute to an agile and skilled IT workforce.</t>
+  </si>
+  <si>
+    <t>The organization establishes a comprehensive quality management framework that covers the entire IT lifecycle. Standardized quality measures, testing protocols, and continuous improvement efforts are documented.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The organization consistently defines and measures quality criteria for IT products and services. Basic quality assurance processes are in place.</t>
+  </si>
+  <si>
+    <t>The organization actively seeks opportunities to enhance quality across IT processes, products, and services. Proactive monitoring, root cause analysis, and innovation contribute to a culture of continuous quality improvement.</t>
+  </si>
+  <si>
+    <t>The organization consistently identifies and assesses IT risks. Basic risk management practices are applied to high-priority areas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The organization establishes a structured risk management framework that covers the full spectrum of IT risks. Risk assessments, mitigation strategies, and risk monitoring mechanisms are documented.</t>
+  </si>
+  <si>
+    <t>The organization actively integrates risk management into all IT activities. Risk awareness, real-time monitoring, and a proactive approach to risk response ensure that IT risks are effectively managed and aligned with business objectives.</t>
+  </si>
+  <si>
+    <t>The organization consistently applies project management practices to IT initiatives. Project progress and outcomes are regularly reviewed.</t>
+  </si>
+  <si>
+    <t>The organization establishes a structured project management methodology that encompasses planning, execution, monitoring, and closure. Standardized project templates, roles, and responsibilities are defined.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The organization actively optimizes its project management practices. Lessons learned, continuous feedback, and the adoption of best practices contribute to efficient project delivery, enhanced outcomes, and stakeholder satisfaction.</t>
   </si>
 </sst>
 </file>
@@ -6999,7 +7091,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="462">
+  <cellXfs count="468">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7659,6 +7751,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8204,87 +8395,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9204,52 +9314,52 @@
       </c>
       <c r="C1" s="218"/>
       <c r="D1" s="218"/>
-      <c r="E1" s="255" t="s">
+      <c r="E1" s="288" t="s">
         <v>663</v>
       </c>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
-      <c r="M1" s="255"/>
-      <c r="N1" s="255"/>
-      <c r="O1" s="255"/>
-      <c r="P1" s="255"/>
-      <c r="Q1" s="255"/>
-      <c r="R1" s="255"/>
-      <c r="S1" s="255"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="288"/>
+      <c r="P1" s="288"/>
+      <c r="Q1" s="288"/>
+      <c r="R1" s="288"/>
+      <c r="S1" s="288"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="123"/>
       <c r="B2" s="217"/>
-      <c r="C2" s="253" t="s">
+      <c r="C2" s="286" t="s">
         <v>572</v>
       </c>
-      <c r="D2" s="254"/>
-      <c r="E2" s="253" t="s">
+      <c r="D2" s="287"/>
+      <c r="E2" s="286" t="s">
         <v>513</v>
       </c>
-      <c r="F2" s="254"/>
+      <c r="F2" s="287"/>
       <c r="G2" s="217"/>
       <c r="H2" s="231"/>
       <c r="I2" s="231"/>
-      <c r="J2" s="256"/>
-      <c r="K2" s="256"/>
-      <c r="L2" s="256"/>
-      <c r="M2" s="256"/>
-      <c r="N2" s="256"/>
-      <c r="O2" s="256"/>
-      <c r="P2" s="256"/>
-      <c r="Q2" s="256"/>
-      <c r="R2" s="256"/>
-      <c r="S2" s="256"/>
-      <c r="T2" s="256"/>
-      <c r="U2" s="256"/>
-      <c r="V2" s="256"/>
-      <c r="W2" s="256"/>
+      <c r="J2" s="289"/>
+      <c r="K2" s="289"/>
+      <c r="L2" s="289"/>
+      <c r="M2" s="289"/>
+      <c r="N2" s="289"/>
+      <c r="O2" s="289"/>
+      <c r="P2" s="289"/>
+      <c r="Q2" s="289"/>
+      <c r="R2" s="289"/>
+      <c r="S2" s="289"/>
+      <c r="T2" s="289"/>
+      <c r="U2" s="289"/>
+      <c r="V2" s="289"/>
+      <c r="W2" s="289"/>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="235" t="s">
@@ -9961,20 +10071,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="46.5" customHeight="1" thickBot="1">
-      <c r="B2" s="370" t="s">
+      <c r="B2" s="403" t="s">
         <v>636</v>
       </c>
-      <c r="C2" s="370"/>
-      <c r="D2" s="370"/>
-      <c r="E2" s="370"/>
+      <c r="C2" s="403"/>
+      <c r="D2" s="403"/>
+      <c r="E2" s="403"/>
     </row>
     <row r="3" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B3" s="367" t="s">
+      <c r="B3" s="400" t="s">
         <v>377</v>
       </c>
-      <c r="C3" s="368"/>
-      <c r="D3" s="368"/>
-      <c r="E3" s="369"/>
+      <c r="C3" s="401"/>
+      <c r="D3" s="401"/>
+      <c r="E3" s="402"/>
       <c r="G3" s="248" t="s">
         <v>779</v>
       </c>
@@ -10055,12 +10165,12 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B11" s="367" t="s">
+      <c r="B11" s="400" t="s">
         <v>775</v>
       </c>
-      <c r="C11" s="368"/>
-      <c r="D11" s="368"/>
-      <c r="E11" s="369"/>
+      <c r="C11" s="401"/>
+      <c r="D11" s="401"/>
+      <c r="E11" s="402"/>
       <c r="G11" s="248" t="s">
         <v>787</v>
       </c>
@@ -10094,7 +10204,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75">
-      <c r="B14" s="361" t="s">
+      <c r="B14" s="394" t="s">
         <v>776</v>
       </c>
       <c r="C14" s="90"/>
@@ -10105,7 +10215,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.75">
-      <c r="B15" s="362"/>
+      <c r="B15" s="395"/>
       <c r="C15" s="92"/>
       <c r="D15" s="204"/>
       <c r="E15" s="93"/>
@@ -10114,7 +10224,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B16" s="363"/>
+      <c r="B16" s="396"/>
       <c r="C16" s="199"/>
       <c r="D16" s="205"/>
       <c r="E16" s="150"/>
@@ -10123,7 +10233,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="15.75">
-      <c r="B17" s="361" t="s">
+      <c r="B17" s="394" t="s">
         <v>777</v>
       </c>
       <c r="C17" s="90"/>
@@ -10134,7 +10244,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75">
-      <c r="B18" s="362"/>
+      <c r="B18" s="395"/>
       <c r="C18" s="92"/>
       <c r="D18" s="204"/>
       <c r="E18" s="191"/>
@@ -10143,7 +10253,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75">
-      <c r="B19" s="362"/>
+      <c r="B19" s="395"/>
       <c r="C19" s="92"/>
       <c r="D19" s="204"/>
       <c r="E19" s="191"/>
@@ -10152,7 +10262,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="15.75">
-      <c r="B20" s="362"/>
+      <c r="B20" s="395"/>
       <c r="C20" s="92"/>
       <c r="D20" s="206"/>
       <c r="E20" s="194"/>
@@ -10161,7 +10271,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B21" s="363"/>
+      <c r="B21" s="396"/>
       <c r="C21" s="199"/>
       <c r="D21" s="205"/>
       <c r="E21" s="150"/>
@@ -10170,7 +10280,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="15.75">
-      <c r="B22" s="361" t="s">
+      <c r="B22" s="394" t="s">
         <v>778</v>
       </c>
       <c r="C22" s="90"/>
@@ -10181,7 +10291,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75">
-      <c r="B23" s="362"/>
+      <c r="B23" s="395"/>
       <c r="C23" s="92"/>
       <c r="D23" s="204"/>
       <c r="E23" s="191"/>
@@ -10190,7 +10300,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75">
-      <c r="B24" s="362"/>
+      <c r="B24" s="395"/>
       <c r="C24" s="92"/>
       <c r="D24" s="204"/>
       <c r="E24" s="191"/>
@@ -10199,7 +10309,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B25" s="363"/>
+      <c r="B25" s="396"/>
       <c r="C25" s="199"/>
       <c r="D25" s="205"/>
       <c r="E25" s="150"/>
@@ -10208,7 +10318,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="15.75">
-      <c r="B26" s="361" t="s">
+      <c r="B26" s="394" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="90"/>
@@ -10219,7 +10329,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="15.75">
-      <c r="B27" s="362"/>
+      <c r="B27" s="395"/>
       <c r="C27" s="92"/>
       <c r="D27" s="204"/>
       <c r="E27" s="191"/>
@@ -10228,7 +10338,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="16.5" thickBot="1">
-      <c r="B28" s="363"/>
+      <c r="B28" s="396"/>
       <c r="C28" s="199"/>
       <c r="D28" s="205"/>
       <c r="E28" s="150"/>
@@ -10852,16 +10962,16 @@
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" thickBot="1">
       <c r="A2" s="130"/>
-      <c r="B2" s="372" t="s">
+      <c r="B2" s="405" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="372" t="s">
+      <c r="C2" s="405" t="s">
         <v>376</v>
       </c>
-      <c r="D2" s="374" t="s">
+      <c r="D2" s="407" t="s">
         <v>482</v>
       </c>
-      <c r="E2" s="375"/>
+      <c r="E2" s="408"/>
       <c r="F2" s="157" t="s">
         <v>485</v>
       </c>
@@ -10875,26 +10985,26 @@
         <v>486</v>
       </c>
       <c r="J2" s="247"/>
-      <c r="K2" s="379" t="s">
+      <c r="K2" s="412" t="s">
         <v>575</v>
       </c>
-      <c r="L2" s="380" t="s">
+      <c r="L2" s="413" t="s">
         <v>595</v>
       </c>
-      <c r="M2" s="381"/>
-      <c r="N2" s="381"/>
-      <c r="O2" s="381"/>
-      <c r="P2" s="381"/>
-      <c r="Q2" s="382"/>
+      <c r="M2" s="414"/>
+      <c r="N2" s="414"/>
+      <c r="O2" s="414"/>
+      <c r="P2" s="414"/>
+      <c r="Q2" s="415"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="130"/>
-      <c r="B3" s="373"/>
-      <c r="C3" s="373"/>
-      <c r="D3" s="374" t="s">
+      <c r="B3" s="406"/>
+      <c r="C3" s="406"/>
+      <c r="D3" s="407" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="376"/>
+      <c r="E3" s="409"/>
       <c r="F3" s="171" t="s">
         <v>101</v>
       </c>
@@ -10908,13 +11018,13 @@
         <v>101</v>
       </c>
       <c r="J3" s="247"/>
-      <c r="K3" s="379"/>
-      <c r="L3" s="383"/>
-      <c r="M3" s="384"/>
-      <c r="N3" s="384"/>
-      <c r="O3" s="384"/>
-      <c r="P3" s="384"/>
-      <c r="Q3" s="385"/>
+      <c r="K3" s="412"/>
+      <c r="L3" s="416"/>
+      <c r="M3" s="417"/>
+      <c r="N3" s="417"/>
+      <c r="O3" s="417"/>
+      <c r="P3" s="417"/>
+      <c r="Q3" s="418"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="130"/>
@@ -10927,13 +11037,13 @@
       <c r="H4" s="130"/>
       <c r="I4" s="130"/>
       <c r="J4" s="130"/>
-      <c r="K4" s="379"/>
-      <c r="L4" s="386"/>
-      <c r="M4" s="387"/>
-      <c r="N4" s="387"/>
-      <c r="O4" s="387"/>
-      <c r="P4" s="387"/>
-      <c r="Q4" s="388"/>
+      <c r="K4" s="412"/>
+      <c r="L4" s="419"/>
+      <c r="M4" s="420"/>
+      <c r="N4" s="420"/>
+      <c r="O4" s="420"/>
+      <c r="P4" s="420"/>
+      <c r="Q4" s="421"/>
     </row>
     <row r="5" spans="1:17" ht="36.6" customHeight="1">
       <c r="A5" s="130"/>
@@ -10963,18 +11073,18 @@
       <c r="K5" s="188" t="s">
         <v>572</v>
       </c>
-      <c r="L5" s="389" t="s">
+      <c r="L5" s="422" t="s">
         <v>576</v>
       </c>
-      <c r="M5" s="390"/>
-      <c r="N5" s="390"/>
-      <c r="O5" s="390"/>
-      <c r="P5" s="390"/>
-      <c r="Q5" s="391"/>
+      <c r="M5" s="423"/>
+      <c r="N5" s="423"/>
+      <c r="O5" s="423"/>
+      <c r="P5" s="423"/>
+      <c r="Q5" s="424"/>
     </row>
     <row r="6" spans="1:17" ht="14.45" customHeight="1">
       <c r="A6" s="130"/>
-      <c r="B6" s="377" t="s">
+      <c r="B6" s="410" t="s">
         <v>572</v>
       </c>
       <c r="C6" s="213" t="s">
@@ -10996,18 +11106,18 @@
       <c r="K6" s="188" t="s">
         <v>513</v>
       </c>
-      <c r="L6" s="389" t="s">
+      <c r="L6" s="422" t="s">
         <v>577</v>
       </c>
-      <c r="M6" s="390"/>
-      <c r="N6" s="390"/>
-      <c r="O6" s="390"/>
-      <c r="P6" s="390"/>
-      <c r="Q6" s="391"/>
+      <c r="M6" s="423"/>
+      <c r="N6" s="423"/>
+      <c r="O6" s="423"/>
+      <c r="P6" s="423"/>
+      <c r="Q6" s="424"/>
     </row>
     <row r="7" spans="1:17" ht="14.45" customHeight="1">
       <c r="A7" s="130"/>
-      <c r="B7" s="378"/>
+      <c r="B7" s="411"/>
       <c r="C7" s="213" t="s">
         <v>641</v>
       </c>
@@ -11027,14 +11137,14 @@
       <c r="K7" s="188" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="389" t="s">
+      <c r="L7" s="422" t="s">
         <v>578</v>
       </c>
-      <c r="M7" s="390"/>
-      <c r="N7" s="390"/>
-      <c r="O7" s="390"/>
-      <c r="P7" s="390"/>
-      <c r="Q7" s="391"/>
+      <c r="M7" s="423"/>
+      <c r="N7" s="423"/>
+      <c r="O7" s="423"/>
+      <c r="P7" s="423"/>
+      <c r="Q7" s="424"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="130"/>
@@ -11062,14 +11172,14 @@
       <c r="K8" s="188" t="s">
         <v>529</v>
       </c>
-      <c r="L8" s="392" t="s">
+      <c r="L8" s="425" t="s">
         <v>579</v>
       </c>
-      <c r="M8" s="393"/>
-      <c r="N8" s="393"/>
-      <c r="O8" s="393"/>
-      <c r="P8" s="393"/>
-      <c r="Q8" s="394"/>
+      <c r="M8" s="426"/>
+      <c r="N8" s="426"/>
+      <c r="O8" s="426"/>
+      <c r="P8" s="426"/>
+      <c r="Q8" s="427"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="130"/>
@@ -11093,14 +11203,14 @@
       <c r="K9" s="188" t="s">
         <v>512</v>
       </c>
-      <c r="L9" s="395" t="s">
+      <c r="L9" s="428" t="s">
         <v>573</v>
       </c>
-      <c r="M9" s="395"/>
-      <c r="N9" s="395"/>
-      <c r="O9" s="395"/>
-      <c r="P9" s="395"/>
-      <c r="Q9" s="395"/>
+      <c r="M9" s="428"/>
+      <c r="N9" s="428"/>
+      <c r="O9" s="428"/>
+      <c r="P9" s="428"/>
+      <c r="Q9" s="428"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="130"/>
@@ -11126,14 +11236,14 @@
       <c r="K10" s="188" t="s">
         <v>377</v>
       </c>
-      <c r="L10" s="395" t="s">
+      <c r="L10" s="428" t="s">
         <v>580</v>
       </c>
-      <c r="M10" s="395"/>
-      <c r="N10" s="395"/>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
-      <c r="Q10" s="395"/>
+      <c r="M10" s="428"/>
+      <c r="N10" s="428"/>
+      <c r="O10" s="428"/>
+      <c r="P10" s="428"/>
+      <c r="Q10" s="428"/>
     </row>
     <row r="11" spans="1:17" ht="14.45" customHeight="1">
       <c r="A11" s="130"/>
@@ -11152,17 +11262,17 @@
       <c r="H11" s="216"/>
       <c r="I11" s="130"/>
       <c r="J11" s="130"/>
-      <c r="K11" s="396" t="s">
+      <c r="K11" s="429" t="s">
         <v>574</v>
       </c>
-      <c r="L11" s="397" t="s">
+      <c r="L11" s="430" t="s">
         <v>599</v>
       </c>
-      <c r="M11" s="398"/>
-      <c r="N11" s="398"/>
-      <c r="O11" s="398"/>
-      <c r="P11" s="398"/>
-      <c r="Q11" s="399"/>
+      <c r="M11" s="431"/>
+      <c r="N11" s="431"/>
+      <c r="O11" s="431"/>
+      <c r="P11" s="431"/>
+      <c r="Q11" s="432"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="130"/>
@@ -11179,13 +11289,13 @@
       <c r="H12" s="216"/>
       <c r="I12" s="130"/>
       <c r="J12" s="130"/>
-      <c r="K12" s="396"/>
-      <c r="L12" s="400"/>
-      <c r="M12" s="401"/>
-      <c r="N12" s="401"/>
-      <c r="O12" s="401"/>
-      <c r="P12" s="401"/>
-      <c r="Q12" s="402"/>
+      <c r="K12" s="429"/>
+      <c r="L12" s="433"/>
+      <c r="M12" s="434"/>
+      <c r="N12" s="434"/>
+      <c r="O12" s="434"/>
+      <c r="P12" s="434"/>
+      <c r="Q12" s="435"/>
     </row>
     <row r="13" spans="1:17" ht="34.5">
       <c r="A13" s="130"/>
@@ -11202,13 +11312,13 @@
       <c r="H13" s="216"/>
       <c r="I13" s="130"/>
       <c r="J13" s="130"/>
-      <c r="K13" s="396"/>
-      <c r="L13" s="403"/>
-      <c r="M13" s="404"/>
-      <c r="N13" s="404"/>
-      <c r="O13" s="404"/>
-      <c r="P13" s="404"/>
-      <c r="Q13" s="405"/>
+      <c r="K13" s="429"/>
+      <c r="L13" s="436"/>
+      <c r="M13" s="437"/>
+      <c r="N13" s="437"/>
+      <c r="O13" s="437"/>
+      <c r="P13" s="437"/>
+      <c r="Q13" s="438"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1">
       <c r="A14" s="130"/>
@@ -11244,14 +11354,14 @@
       <c r="I15" s="130"/>
       <c r="J15" s="130"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="371" t="s">
+      <c r="L15" s="404" t="s">
         <v>594</v>
       </c>
-      <c r="M15" s="371"/>
-      <c r="N15" s="371"/>
-      <c r="O15" s="371"/>
-      <c r="P15" s="371"/>
-      <c r="Q15" s="371"/>
+      <c r="M15" s="404"/>
+      <c r="N15" s="404"/>
+      <c r="O15" s="404"/>
+      <c r="P15" s="404"/>
+      <c r="Q15" s="404"/>
     </row>
     <row r="16" spans="1:17" ht="21" customHeight="1">
       <c r="A16" s="130"/>
@@ -11268,115 +11378,115 @@
       <c r="H16" s="216"/>
       <c r="I16" s="130"/>
       <c r="J16" s="130"/>
-      <c r="K16" s="406" t="s">
+      <c r="K16" s="439" t="s">
         <v>581</v>
       </c>
       <c r="L16" s="246" t="s">
         <v>588</v>
       </c>
-      <c r="M16" s="407" t="s">
+      <c r="M16" s="440" t="s">
         <v>582</v>
       </c>
-      <c r="N16" s="407"/>
-      <c r="O16" s="407"/>
-      <c r="P16" s="407"/>
-      <c r="Q16" s="407"/>
+      <c r="N16" s="440"/>
+      <c r="O16" s="440"/>
+      <c r="P16" s="440"/>
+      <c r="Q16" s="440"/>
     </row>
     <row r="17" spans="8:17" ht="18" customHeight="1">
       <c r="H17" s="130"/>
       <c r="I17" s="130"/>
       <c r="J17" s="130"/>
-      <c r="K17" s="406"/>
+      <c r="K17" s="439"/>
       <c r="L17" s="246" t="s">
         <v>589</v>
       </c>
-      <c r="M17" s="407" t="s">
+      <c r="M17" s="440" t="s">
         <v>583</v>
       </c>
-      <c r="N17" s="407"/>
-      <c r="O17" s="407"/>
-      <c r="P17" s="407"/>
-      <c r="Q17" s="407"/>
+      <c r="N17" s="440"/>
+      <c r="O17" s="440"/>
+      <c r="P17" s="440"/>
+      <c r="Q17" s="440"/>
     </row>
     <row r="18" spans="8:17" ht="18" customHeight="1">
       <c r="H18" s="130"/>
       <c r="I18" s="130"/>
       <c r="J18" s="130"/>
-      <c r="K18" s="406"/>
+      <c r="K18" s="439"/>
       <c r="L18" s="246" t="s">
         <v>596</v>
       </c>
-      <c r="M18" s="408" t="s">
+      <c r="M18" s="441" t="s">
         <v>597</v>
       </c>
-      <c r="N18" s="407"/>
-      <c r="O18" s="407"/>
-      <c r="P18" s="407"/>
-      <c r="Q18" s="407"/>
+      <c r="N18" s="440"/>
+      <c r="O18" s="440"/>
+      <c r="P18" s="440"/>
+      <c r="Q18" s="440"/>
     </row>
     <row r="19" spans="8:17" ht="18" customHeight="1">
       <c r="H19" s="130"/>
       <c r="I19" s="130"/>
       <c r="J19" s="130"/>
-      <c r="K19" s="406"/>
+      <c r="K19" s="439"/>
       <c r="L19" s="246" t="s">
         <v>590</v>
       </c>
-      <c r="M19" s="407" t="s">
+      <c r="M19" s="440" t="s">
         <v>584</v>
       </c>
-      <c r="N19" s="407"/>
-      <c r="O19" s="407"/>
-      <c r="P19" s="407"/>
-      <c r="Q19" s="407"/>
+      <c r="N19" s="440"/>
+      <c r="O19" s="440"/>
+      <c r="P19" s="440"/>
+      <c r="Q19" s="440"/>
     </row>
     <row r="20" spans="8:17" ht="18" customHeight="1">
       <c r="H20" s="130"/>
       <c r="I20" s="130"/>
       <c r="J20" s="130"/>
-      <c r="K20" s="406"/>
+      <c r="K20" s="439"/>
       <c r="L20" s="246" t="s">
         <v>591</v>
       </c>
-      <c r="M20" s="407" t="s">
+      <c r="M20" s="440" t="s">
         <v>585</v>
       </c>
-      <c r="N20" s="407"/>
-      <c r="O20" s="407"/>
-      <c r="P20" s="407"/>
-      <c r="Q20" s="407"/>
+      <c r="N20" s="440"/>
+      <c r="O20" s="440"/>
+      <c r="P20" s="440"/>
+      <c r="Q20" s="440"/>
     </row>
     <row r="21" spans="8:17" ht="18" customHeight="1">
       <c r="H21" s="130"/>
       <c r="I21" s="130"/>
       <c r="J21" s="130"/>
-      <c r="K21" s="406"/>
+      <c r="K21" s="439"/>
       <c r="L21" s="246" t="s">
         <v>592</v>
       </c>
-      <c r="M21" s="407" t="s">
+      <c r="M21" s="440" t="s">
         <v>586</v>
       </c>
-      <c r="N21" s="407"/>
-      <c r="O21" s="407"/>
-      <c r="P21" s="407"/>
-      <c r="Q21" s="407"/>
+      <c r="N21" s="440"/>
+      <c r="O21" s="440"/>
+      <c r="P21" s="440"/>
+      <c r="Q21" s="440"/>
     </row>
     <row r="22" spans="8:17" ht="18" customHeight="1">
       <c r="H22" s="130"/>
       <c r="I22" s="130"/>
       <c r="J22" s="130"/>
-      <c r="K22" s="406"/>
+      <c r="K22" s="439"/>
       <c r="L22" s="246" t="s">
         <v>593</v>
       </c>
-      <c r="M22" s="407" t="s">
+      <c r="M22" s="440" t="s">
         <v>587</v>
       </c>
-      <c r="N22" s="407"/>
-      <c r="O22" s="407"/>
-      <c r="P22" s="407"/>
-      <c r="Q22" s="407"/>
+      <c r="N22" s="440"/>
+      <c r="O22" s="440"/>
+      <c r="P22" s="440"/>
+      <c r="Q22" s="440"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -11414,7 +11524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -11610,14 +11720,14 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1">
       <c r="B2" s="145"/>
-      <c r="C2" s="424" t="s">
+      <c r="C2" s="457" t="s">
         <v>556</v>
       </c>
-      <c r="D2" s="424"/>
-      <c r="E2" s="424"/>
-      <c r="F2" s="424"/>
-      <c r="G2" s="424"/>
-      <c r="H2" s="425"/>
+      <c r="D2" s="457"/>
+      <c r="E2" s="457"/>
+      <c r="F2" s="457"/>
+      <c r="G2" s="457"/>
+      <c r="H2" s="458"/>
       <c r="K2" t="s">
         <v>644</v>
       </c>
@@ -11626,105 +11736,105 @@
       <c r="B3" s="145" t="s">
         <v>475</v>
       </c>
-      <c r="C3" s="431" t="s">
+      <c r="C3" s="464" t="s">
         <v>920</v>
       </c>
-      <c r="D3" s="432"/>
-      <c r="E3" s="432"/>
-      <c r="F3" s="432"/>
-      <c r="G3" s="432"/>
-      <c r="H3" s="433"/>
+      <c r="D3" s="465"/>
+      <c r="E3" s="465"/>
+      <c r="F3" s="465"/>
+      <c r="G3" s="465"/>
+      <c r="H3" s="466"/>
     </row>
     <row r="4" spans="2:11" ht="25.5" customHeight="1" thickBot="1">
       <c r="B4" s="250" t="s">
         <v>489</v>
       </c>
-      <c r="C4" s="434" t="s">
+      <c r="C4" s="467" t="s">
         <v>922</v>
       </c>
-      <c r="D4" s="434"/>
-      <c r="E4" s="434"/>
-      <c r="F4" s="434"/>
-      <c r="G4" s="434"/>
-      <c r="H4" s="434"/>
+      <c r="D4" s="467"/>
+      <c r="E4" s="467"/>
+      <c r="F4" s="467"/>
+      <c r="G4" s="467"/>
+      <c r="H4" s="467"/>
     </row>
     <row r="5" spans="2:11" ht="25.5" customHeight="1" thickBot="1">
       <c r="B5" s="250" t="s">
         <v>488</v>
       </c>
-      <c r="C5" s="434" t="s">
+      <c r="C5" s="467" t="s">
         <v>560</v>
       </c>
-      <c r="D5" s="434"/>
-      <c r="E5" s="434"/>
-      <c r="F5" s="434"/>
-      <c r="G5" s="434"/>
-      <c r="H5" s="434"/>
+      <c r="D5" s="467"/>
+      <c r="E5" s="467"/>
+      <c r="F5" s="467"/>
+      <c r="G5" s="467"/>
+      <c r="H5" s="467"/>
     </row>
     <row r="6" spans="2:11" ht="23.25" customHeight="1" thickBot="1">
       <c r="B6" s="250" t="s">
         <v>557</v>
       </c>
-      <c r="C6" s="434" t="s">
+      <c r="C6" s="467" t="s">
         <v>473</v>
       </c>
-      <c r="D6" s="434"/>
-      <c r="E6" s="434"/>
-      <c r="F6" s="434"/>
-      <c r="G6" s="434"/>
-      <c r="H6" s="434"/>
+      <c r="D6" s="467"/>
+      <c r="E6" s="467"/>
+      <c r="F6" s="467"/>
+      <c r="G6" s="467"/>
+      <c r="H6" s="467"/>
     </row>
     <row r="7" spans="2:11" ht="23.25" customHeight="1" thickBot="1">
       <c r="B7" s="250" t="s">
         <v>476</v>
       </c>
-      <c r="C7" s="434" t="s">
+      <c r="C7" s="467" t="s">
         <v>473</v>
       </c>
-      <c r="D7" s="434"/>
-      <c r="E7" s="434"/>
-      <c r="F7" s="434"/>
-      <c r="G7" s="434"/>
-      <c r="H7" s="434"/>
+      <c r="D7" s="467"/>
+      <c r="E7" s="467"/>
+      <c r="F7" s="467"/>
+      <c r="G7" s="467"/>
+      <c r="H7" s="467"/>
     </row>
     <row r="8" spans="2:11" ht="23.25" customHeight="1" thickBot="1">
       <c r="B8" s="250" t="s">
         <v>558</v>
       </c>
-      <c r="C8" s="434" t="s">
+      <c r="C8" s="467" t="s">
         <v>918</v>
       </c>
-      <c r="D8" s="434"/>
-      <c r="E8" s="434"/>
-      <c r="F8" s="434"/>
-      <c r="G8" s="434"/>
-      <c r="H8" s="434"/>
+      <c r="D8" s="467"/>
+      <c r="E8" s="467"/>
+      <c r="F8" s="467"/>
+      <c r="G8" s="467"/>
+      <c r="H8" s="467"/>
     </row>
     <row r="9" spans="2:11" ht="23.25" customHeight="1" thickBot="1">
       <c r="B9" s="250" t="s">
         <v>495</v>
       </c>
-      <c r="C9" s="434" t="s">
+      <c r="C9" s="467" t="s">
         <v>474</v>
       </c>
-      <c r="D9" s="434"/>
-      <c r="E9" s="434"/>
-      <c r="F9" s="434"/>
-      <c r="G9" s="434"/>
-      <c r="H9" s="434"/>
+      <c r="D9" s="467"/>
+      <c r="E9" s="467"/>
+      <c r="F9" s="467"/>
+      <c r="G9" s="467"/>
+      <c r="H9" s="467"/>
     </row>
     <row r="10" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B10" s="250" t="s">
         <v>559</v>
       </c>
-      <c r="C10" s="434" t="s">
+      <c r="C10" s="467" t="s">
         <v>921</v>
       </c>
-      <c r="D10" s="434"/>
-      <c r="E10" s="434"/>
-      <c r="F10" s="434"/>
-      <c r="G10" s="434"/>
-      <c r="H10" s="434"/>
+      <c r="D10" s="467"/>
+      <c r="E10" s="467"/>
+      <c r="F10" s="467"/>
+      <c r="G10" s="467"/>
+      <c r="H10" s="467"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1">
       <c r="B11" s="123"/>
@@ -11736,13 +11846,13 @@
       <c r="H11" s="123"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B12" s="421" t="s">
+      <c r="B12" s="454" t="s">
         <v>498</v>
       </c>
-      <c r="C12" s="422"/>
-      <c r="D12" s="422"/>
-      <c r="E12" s="422"/>
-      <c r="F12" s="423"/>
+      <c r="C12" s="455"/>
+      <c r="D12" s="455"/>
+      <c r="E12" s="455"/>
+      <c r="F12" s="456"/>
       <c r="G12" s="251"/>
       <c r="H12" s="147"/>
     </row>
@@ -11750,13 +11860,13 @@
       <c r="B13" s="145" t="s">
         <v>475</v>
       </c>
-      <c r="C13" s="415" t="s">
+      <c r="C13" s="448" t="s">
         <v>919</v>
       </c>
-      <c r="D13" s="416"/>
-      <c r="E13" s="416"/>
-      <c r="F13" s="416"/>
-      <c r="G13" s="417"/>
+      <c r="D13" s="449"/>
+      <c r="E13" s="449"/>
+      <c r="F13" s="449"/>
+      <c r="G13" s="450"/>
       <c r="H13" s="145">
         <v>7</v>
       </c>
@@ -11765,13 +11875,13 @@
       <c r="B14" s="148" t="s">
         <v>489</v>
       </c>
-      <c r="C14" s="415" t="s">
+      <c r="C14" s="448" t="s">
         <v>494</v>
       </c>
-      <c r="D14" s="416"/>
-      <c r="E14" s="416"/>
-      <c r="F14" s="416"/>
-      <c r="G14" s="417"/>
+      <c r="D14" s="449"/>
+      <c r="E14" s="449"/>
+      <c r="F14" s="449"/>
+      <c r="G14" s="450"/>
       <c r="H14" s="145">
         <v>12</v>
       </c>
@@ -11780,13 +11890,13 @@
       <c r="B15" s="146" t="s">
         <v>488</v>
       </c>
-      <c r="C15" s="415" t="s">
+      <c r="C15" s="448" t="s">
         <v>493</v>
       </c>
-      <c r="D15" s="416"/>
-      <c r="E15" s="416"/>
-      <c r="F15" s="416"/>
-      <c r="G15" s="417"/>
+      <c r="D15" s="449"/>
+      <c r="E15" s="449"/>
+      <c r="F15" s="449"/>
+      <c r="G15" s="450"/>
       <c r="H15" s="145">
         <v>6</v>
       </c>
@@ -11795,13 +11905,13 @@
       <c r="B16" s="146" t="s">
         <v>491</v>
       </c>
-      <c r="C16" s="415" t="s">
+      <c r="C16" s="448" t="s">
         <v>492</v>
       </c>
-      <c r="D16" s="416"/>
-      <c r="E16" s="416"/>
-      <c r="F16" s="416"/>
-      <c r="G16" s="417"/>
+      <c r="D16" s="449"/>
+      <c r="E16" s="449"/>
+      <c r="F16" s="449"/>
+      <c r="G16" s="450"/>
       <c r="H16" s="145">
         <v>10</v>
       </c>
@@ -11810,13 +11920,13 @@
       <c r="B17" s="87" t="s">
         <v>490</v>
       </c>
-      <c r="C17" s="415" t="s">
+      <c r="C17" s="448" t="s">
         <v>499</v>
       </c>
-      <c r="D17" s="416"/>
-      <c r="E17" s="416"/>
-      <c r="F17" s="416"/>
-      <c r="G17" s="417"/>
+      <c r="D17" s="449"/>
+      <c r="E17" s="449"/>
+      <c r="F17" s="449"/>
+      <c r="G17" s="450"/>
       <c r="H17" s="145">
         <v>13</v>
       </c>
@@ -11825,13 +11935,13 @@
       <c r="B18" s="87" t="s">
         <v>496</v>
       </c>
-      <c r="C18" s="415" t="s">
+      <c r="C18" s="448" t="s">
         <v>497</v>
       </c>
-      <c r="D18" s="416"/>
-      <c r="E18" s="416"/>
-      <c r="F18" s="416"/>
-      <c r="G18" s="417"/>
+      <c r="D18" s="449"/>
+      <c r="E18" s="449"/>
+      <c r="F18" s="449"/>
+      <c r="G18" s="450"/>
       <c r="H18" s="145">
         <v>4</v>
       </c>
@@ -11840,13 +11950,13 @@
       <c r="B19" s="87" t="s">
         <v>495</v>
       </c>
-      <c r="C19" s="415" t="s">
+      <c r="C19" s="448" t="s">
         <v>500</v>
       </c>
-      <c r="D19" s="416"/>
-      <c r="E19" s="416"/>
-      <c r="F19" s="416"/>
-      <c r="G19" s="417"/>
+      <c r="D19" s="449"/>
+      <c r="E19" s="449"/>
+      <c r="F19" s="449"/>
+      <c r="G19" s="450"/>
       <c r="H19" s="145">
         <v>11</v>
       </c>
@@ -11855,13 +11965,13 @@
       <c r="B20" s="145" t="s">
         <v>477</v>
       </c>
-      <c r="C20" s="415" t="s">
+      <c r="C20" s="448" t="s">
         <v>545</v>
       </c>
-      <c r="D20" s="416"/>
-      <c r="E20" s="416"/>
-      <c r="F20" s="416"/>
-      <c r="G20" s="417"/>
+      <c r="D20" s="449"/>
+      <c r="E20" s="449"/>
+      <c r="F20" s="449"/>
+      <c r="G20" s="450"/>
       <c r="H20" s="145">
         <v>5</v>
       </c>
@@ -11879,110 +11989,110 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B22" s="418" t="s">
+      <c r="B22" s="451" t="s">
         <v>487</v>
       </c>
-      <c r="C22" s="419"/>
-      <c r="D22" s="419"/>
-      <c r="E22" s="419"/>
-      <c r="F22" s="419"/>
-      <c r="G22" s="419"/>
-      <c r="H22" s="420"/>
+      <c r="C22" s="452"/>
+      <c r="D22" s="452"/>
+      <c r="E22" s="452"/>
+      <c r="F22" s="452"/>
+      <c r="G22" s="452"/>
+      <c r="H22" s="453"/>
     </row>
     <row r="23" spans="2:8" ht="14.45" customHeight="1">
-      <c r="B23" s="426" t="s">
+      <c r="B23" s="459" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="409" t="s">
+      <c r="C23" s="442" t="s">
         <v>501</v>
       </c>
-      <c r="D23" s="410"/>
-      <c r="E23" s="410"/>
-      <c r="F23" s="410"/>
-      <c r="G23" s="410"/>
-      <c r="H23" s="411"/>
+      <c r="D23" s="443"/>
+      <c r="E23" s="443"/>
+      <c r="F23" s="443"/>
+      <c r="G23" s="443"/>
+      <c r="H23" s="444"/>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B24" s="428"/>
-      <c r="C24" s="409"/>
-      <c r="D24" s="410"/>
-      <c r="E24" s="410"/>
-      <c r="F24" s="410"/>
-      <c r="G24" s="410"/>
-      <c r="H24" s="411"/>
+      <c r="B24" s="461"/>
+      <c r="C24" s="442"/>
+      <c r="D24" s="443"/>
+      <c r="E24" s="443"/>
+      <c r="F24" s="443"/>
+      <c r="G24" s="443"/>
+      <c r="H24" s="444"/>
     </row>
     <row r="25" spans="2:8" ht="14.45" customHeight="1">
-      <c r="B25" s="426" t="s">
+      <c r="B25" s="459" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="409"/>
-      <c r="D25" s="410"/>
-      <c r="E25" s="410"/>
-      <c r="F25" s="410"/>
-      <c r="G25" s="410"/>
-      <c r="H25" s="411"/>
+      <c r="C25" s="442"/>
+      <c r="D25" s="443"/>
+      <c r="E25" s="443"/>
+      <c r="F25" s="443"/>
+      <c r="G25" s="443"/>
+      <c r="H25" s="444"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B26" s="428"/>
-      <c r="C26" s="409"/>
-      <c r="D26" s="410"/>
-      <c r="E26" s="410"/>
-      <c r="F26" s="410"/>
-      <c r="G26" s="410"/>
-      <c r="H26" s="411"/>
+      <c r="B26" s="461"/>
+      <c r="C26" s="442"/>
+      <c r="D26" s="443"/>
+      <c r="E26" s="443"/>
+      <c r="F26" s="443"/>
+      <c r="G26" s="443"/>
+      <c r="H26" s="444"/>
     </row>
     <row r="27" spans="2:8" ht="14.45" customHeight="1">
-      <c r="B27" s="429" t="s">
+      <c r="B27" s="462" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="409" t="s">
+      <c r="C27" s="442" t="s">
         <v>502</v>
       </c>
-      <c r="D27" s="410"/>
-      <c r="E27" s="410"/>
-      <c r="F27" s="410"/>
-      <c r="G27" s="410"/>
-      <c r="H27" s="411"/>
+      <c r="D27" s="443"/>
+      <c r="E27" s="443"/>
+      <c r="F27" s="443"/>
+      <c r="G27" s="443"/>
+      <c r="H27" s="444"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B28" s="430"/>
-      <c r="C28" s="409"/>
-      <c r="D28" s="410"/>
-      <c r="E28" s="410"/>
-      <c r="F28" s="410"/>
-      <c r="G28" s="410"/>
-      <c r="H28" s="411"/>
+      <c r="B28" s="463"/>
+      <c r="C28" s="442"/>
+      <c r="D28" s="443"/>
+      <c r="E28" s="443"/>
+      <c r="F28" s="443"/>
+      <c r="G28" s="443"/>
+      <c r="H28" s="444"/>
     </row>
     <row r="29" spans="2:8" ht="14.45" customHeight="1">
-      <c r="B29" s="426" t="s">
+      <c r="B29" s="459" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="409" t="s">
+      <c r="C29" s="442" t="s">
         <v>503</v>
       </c>
-      <c r="D29" s="410"/>
-      <c r="E29" s="410"/>
-      <c r="F29" s="410"/>
-      <c r="G29" s="410"/>
-      <c r="H29" s="411"/>
+      <c r="D29" s="443"/>
+      <c r="E29" s="443"/>
+      <c r="F29" s="443"/>
+      <c r="G29" s="443"/>
+      <c r="H29" s="444"/>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="427"/>
-      <c r="C30" s="409"/>
-      <c r="D30" s="410"/>
-      <c r="E30" s="410"/>
-      <c r="F30" s="410"/>
-      <c r="G30" s="410"/>
-      <c r="H30" s="411"/>
+      <c r="B30" s="460"/>
+      <c r="C30" s="442"/>
+      <c r="D30" s="443"/>
+      <c r="E30" s="443"/>
+      <c r="F30" s="443"/>
+      <c r="G30" s="443"/>
+      <c r="H30" s="444"/>
     </row>
     <row r="31" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B31" s="428"/>
-      <c r="C31" s="412"/>
-      <c r="D31" s="413"/>
-      <c r="E31" s="413"/>
-      <c r="F31" s="413"/>
-      <c r="G31" s="413"/>
-      <c r="H31" s="414"/>
+      <c r="B31" s="461"/>
+      <c r="C31" s="445"/>
+      <c r="D31" s="446"/>
+      <c r="E31" s="446"/>
+      <c r="F31" s="446"/>
+      <c r="G31" s="446"/>
+      <c r="H31" s="447"/>
     </row>
     <row r="32" spans="2:8">
       <c r="H32" s="184"/>
@@ -12057,23 +12167,23 @@
         <v>664</v>
       </c>
       <c r="C1" s="218"/>
-      <c r="D1" s="255" t="s">
+      <c r="D1" s="288" t="s">
         <v>663</v>
       </c>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
-      <c r="M1" s="255"/>
-      <c r="N1" s="255"/>
-      <c r="O1" s="255"/>
-      <c r="P1" s="255"/>
-      <c r="Q1" s="255"/>
-      <c r="R1" s="255"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="288"/>
+      <c r="P1" s="288"/>
+      <c r="Q1" s="288"/>
+      <c r="R1" s="288"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
@@ -12094,36 +12204,36 @@
       <c r="F2" s="217" t="s">
         <v>653</v>
       </c>
-      <c r="G2" s="256" t="s">
+      <c r="G2" s="289" t="s">
         <v>654</v>
       </c>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256" t="s">
+      <c r="H2" s="289"/>
+      <c r="I2" s="289" t="s">
         <v>657</v>
       </c>
-      <c r="J2" s="256"/>
-      <c r="K2" s="256" t="s">
+      <c r="J2" s="289"/>
+      <c r="K2" s="289" t="s">
         <v>659</v>
       </c>
-      <c r="L2" s="256"/>
-      <c r="M2" s="256" t="s">
+      <c r="L2" s="289"/>
+      <c r="M2" s="289" t="s">
         <v>660</v>
       </c>
-      <c r="N2" s="256"/>
-      <c r="O2" s="256" t="s">
+      <c r="N2" s="289"/>
+      <c r="O2" s="289" t="s">
         <v>661</v>
       </c>
-      <c r="P2" s="256"/>
-      <c r="Q2" s="256" t="s">
+      <c r="P2" s="289"/>
+      <c r="Q2" s="289" t="s">
         <v>671</v>
       </c>
-      <c r="R2" s="256"/>
-      <c r="S2" s="256" t="s">
+      <c r="R2" s="289"/>
+      <c r="S2" s="289" t="s">
         <v>662</v>
       </c>
-      <c r="T2" s="256"/>
-      <c r="U2" s="256"/>
-      <c r="V2" s="256"/>
+      <c r="T2" s="289"/>
+      <c r="U2" s="289"/>
+      <c r="V2" s="289"/>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="236" t="s">
@@ -12835,56 +12945,56 @@
   <sheetData>
     <row r="1" spans="2:10" ht="12.75" thickBot="1"/>
     <row r="2" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B2" s="257" t="s">
+      <c r="B2" s="290" t="s">
         <v>566</v>
       </c>
-      <c r="C2" s="257" t="s">
+      <c r="C2" s="290" t="s">
         <v>770</v>
       </c>
       <c r="D2" s="151" t="s">
         <v>460</v>
       </c>
-      <c r="E2" s="266" t="s">
+      <c r="E2" s="299" t="s">
         <v>458</v>
       </c>
-      <c r="F2" s="267"/>
-      <c r="G2" s="267"/>
-      <c r="H2" s="267"/>
-      <c r="I2" s="267"/>
-      <c r="J2" s="268"/>
+      <c r="F2" s="300"/>
+      <c r="G2" s="300"/>
+      <c r="H2" s="300"/>
+      <c r="I2" s="300"/>
+      <c r="J2" s="301"/>
     </row>
     <row r="3" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B3" s="258"/>
-      <c r="C3" s="258"/>
-      <c r="D3" s="262">
+      <c r="B3" s="291"/>
+      <c r="C3" s="291"/>
+      <c r="D3" s="295">
         <v>1</v>
       </c>
-      <c r="E3" s="269" t="s">
+      <c r="E3" s="302" t="s">
         <v>466</v>
       </c>
-      <c r="F3" s="270"/>
-      <c r="G3" s="270"/>
-      <c r="H3" s="270"/>
-      <c r="I3" s="270"/>
-      <c r="J3" s="271"/>
+      <c r="F3" s="303"/>
+      <c r="G3" s="303"/>
+      <c r="H3" s="303"/>
+      <c r="I3" s="303"/>
+      <c r="J3" s="304"/>
     </row>
     <row r="4" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B4" s="258"/>
-      <c r="C4" s="258"/>
-      <c r="D4" s="262"/>
-      <c r="E4" s="278" t="s">
+      <c r="B4" s="291"/>
+      <c r="C4" s="291"/>
+      <c r="D4" s="295"/>
+      <c r="E4" s="311" t="s">
         <v>506</v>
       </c>
-      <c r="F4" s="279"/>
-      <c r="G4" s="279"/>
-      <c r="H4" s="279"/>
-      <c r="I4" s="279"/>
-      <c r="J4" s="280"/>
+      <c r="F4" s="312"/>
+      <c r="G4" s="312"/>
+      <c r="H4" s="312"/>
+      <c r="I4" s="312"/>
+      <c r="J4" s="313"/>
     </row>
     <row r="5" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B5" s="258"/>
-      <c r="C5" s="258"/>
-      <c r="D5" s="262"/>
+      <c r="B5" s="291"/>
+      <c r="C5" s="291"/>
+      <c r="D5" s="295"/>
       <c r="E5" s="152" t="s">
         <v>435</v>
       </c>
@@ -12905,187 +13015,187 @@
       </c>
     </row>
     <row r="6" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B6" s="258"/>
-      <c r="C6" s="258"/>
-      <c r="D6" s="262"/>
-      <c r="E6" s="284" t="s">
+      <c r="B6" s="291"/>
+      <c r="C6" s="291"/>
+      <c r="D6" s="295"/>
+      <c r="E6" s="317" t="s">
         <v>923</v>
       </c>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285"/>
-      <c r="H6" s="285"/>
-      <c r="I6" s="285"/>
-      <c r="J6" s="286"/>
+      <c r="F6" s="318"/>
+      <c r="G6" s="318"/>
+      <c r="H6" s="318"/>
+      <c r="I6" s="318"/>
+      <c r="J6" s="319"/>
     </row>
     <row r="7" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="258"/>
-      <c r="C7" s="258"/>
-      <c r="D7" s="262"/>
-      <c r="E7" s="284" t="s">
+      <c r="B7" s="291"/>
+      <c r="C7" s="291"/>
+      <c r="D7" s="295"/>
+      <c r="E7" s="317" t="s">
         <v>439</v>
       </c>
-      <c r="F7" s="285"/>
-      <c r="G7" s="288"/>
-      <c r="H7" s="295" t="s">
+      <c r="F7" s="318"/>
+      <c r="G7" s="321"/>
+      <c r="H7" s="328" t="s">
         <v>438</v>
       </c>
-      <c r="I7" s="279"/>
-      <c r="J7" s="280"/>
+      <c r="I7" s="312"/>
+      <c r="J7" s="313"/>
     </row>
     <row r="8" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="258"/>
-      <c r="C8" s="258"/>
-      <c r="D8" s="262"/>
-      <c r="E8" s="269" t="s">
+      <c r="B8" s="291"/>
+      <c r="C8" s="291"/>
+      <c r="D8" s="295"/>
+      <c r="E8" s="302" t="s">
         <v>464</v>
       </c>
-      <c r="F8" s="270"/>
-      <c r="G8" s="270"/>
-      <c r="H8" s="270"/>
-      <c r="I8" s="270"/>
-      <c r="J8" s="271"/>
+      <c r="F8" s="303"/>
+      <c r="G8" s="303"/>
+      <c r="H8" s="303"/>
+      <c r="I8" s="303"/>
+      <c r="J8" s="304"/>
     </row>
     <row r="9" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B9" s="258"/>
-      <c r="C9" s="258"/>
-      <c r="D9" s="263"/>
-      <c r="E9" s="274" t="s">
+      <c r="B9" s="291"/>
+      <c r="C9" s="291"/>
+      <c r="D9" s="296"/>
+      <c r="E9" s="307" t="s">
         <v>505</v>
       </c>
-      <c r="F9" s="275"/>
-      <c r="G9" s="275"/>
-      <c r="H9" s="275"/>
-      <c r="I9" s="275"/>
-      <c r="J9" s="276"/>
+      <c r="F9" s="308"/>
+      <c r="G9" s="308"/>
+      <c r="H9" s="308"/>
+      <c r="I9" s="308"/>
+      <c r="J9" s="309"/>
     </row>
     <row r="10" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B10" s="258"/>
-      <c r="C10" s="258"/>
-      <c r="D10" s="291">
+      <c r="B10" s="291"/>
+      <c r="C10" s="291"/>
+      <c r="D10" s="324">
         <v>2</v>
       </c>
-      <c r="E10" s="269" t="s">
+      <c r="E10" s="302" t="s">
         <v>571</v>
       </c>
-      <c r="F10" s="270"/>
-      <c r="G10" s="270"/>
-      <c r="H10" s="270"/>
-      <c r="I10" s="270"/>
-      <c r="J10" s="271"/>
+      <c r="F10" s="303"/>
+      <c r="G10" s="303"/>
+      <c r="H10" s="303"/>
+      <c r="I10" s="303"/>
+      <c r="J10" s="304"/>
     </row>
     <row r="11" spans="2:10" s="115" customFormat="1" ht="15" customHeight="1">
-      <c r="B11" s="258"/>
-      <c r="C11" s="258"/>
-      <c r="D11" s="291"/>
-      <c r="E11" s="272" t="s">
+      <c r="B11" s="291"/>
+      <c r="C11" s="291"/>
+      <c r="D11" s="324"/>
+      <c r="E11" s="305" t="s">
         <v>445</v>
       </c>
-      <c r="F11" s="261"/>
-      <c r="G11" s="261"/>
-      <c r="H11" s="261"/>
-      <c r="I11" s="261"/>
-      <c r="J11" s="273"/>
+      <c r="F11" s="294"/>
+      <c r="G11" s="294"/>
+      <c r="H11" s="294"/>
+      <c r="I11" s="294"/>
+      <c r="J11" s="306"/>
     </row>
     <row r="12" spans="2:10" s="115" customFormat="1" ht="26.45" customHeight="1">
-      <c r="B12" s="258"/>
-      <c r="C12" s="258"/>
-      <c r="D12" s="291"/>
-      <c r="E12" s="277" t="s">
+      <c r="B12" s="291"/>
+      <c r="C12" s="291"/>
+      <c r="D12" s="324"/>
+      <c r="E12" s="310" t="s">
         <v>567</v>
       </c>
-      <c r="F12" s="277"/>
-      <c r="G12" s="277"/>
-      <c r="H12" s="277" t="s">
+      <c r="F12" s="310"/>
+      <c r="G12" s="310"/>
+      <c r="H12" s="310" t="s">
         <v>569</v>
       </c>
-      <c r="I12" s="277"/>
-      <c r="J12" s="277"/>
+      <c r="I12" s="310"/>
+      <c r="J12" s="310"/>
     </row>
     <row r="13" spans="2:10" s="115" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B13" s="259"/>
-      <c r="C13" s="259"/>
-      <c r="D13" s="291"/>
-      <c r="E13" s="281" t="s">
+      <c r="B13" s="292"/>
+      <c r="C13" s="292"/>
+      <c r="D13" s="324"/>
+      <c r="E13" s="314" t="s">
         <v>769</v>
       </c>
-      <c r="F13" s="282"/>
-      <c r="G13" s="282"/>
-      <c r="H13" s="282"/>
-      <c r="I13" s="282"/>
-      <c r="J13" s="283"/>
+      <c r="F13" s="315"/>
+      <c r="G13" s="315"/>
+      <c r="H13" s="315"/>
+      <c r="I13" s="315"/>
+      <c r="J13" s="316"/>
     </row>
     <row r="14" spans="2:10" s="115" customFormat="1" ht="25.5" customHeight="1">
       <c r="B14" s="116"/>
       <c r="C14" s="117"/>
       <c r="D14" s="117"/>
-      <c r="E14" s="261" t="s">
+      <c r="E14" s="294" t="s">
         <v>462</v>
       </c>
-      <c r="F14" s="261"/>
-      <c r="G14" s="261"/>
-      <c r="H14" s="261"/>
-      <c r="I14" s="261"/>
-      <c r="J14" s="261"/>
+      <c r="F14" s="294"/>
+      <c r="G14" s="294"/>
+      <c r="H14" s="294"/>
+      <c r="I14" s="294"/>
+      <c r="J14" s="294"/>
     </row>
     <row r="15" spans="2:10" s="115" customFormat="1" ht="24.95" customHeight="1">
-      <c r="B15" s="260" t="s">
+      <c r="B15" s="293" t="s">
         <v>637</v>
       </c>
-      <c r="C15" s="260" t="s">
+      <c r="C15" s="293" t="s">
         <v>440</v>
       </c>
-      <c r="D15" s="292">
+      <c r="D15" s="325">
         <v>3</v>
       </c>
-      <c r="E15" s="277" t="s">
+      <c r="E15" s="310" t="s">
         <v>568</v>
       </c>
-      <c r="F15" s="277"/>
-      <c r="G15" s="277"/>
-      <c r="H15" s="277"/>
-      <c r="I15" s="277"/>
-      <c r="J15" s="277"/>
+      <c r="F15" s="310"/>
+      <c r="G15" s="310"/>
+      <c r="H15" s="310"/>
+      <c r="I15" s="310"/>
+      <c r="J15" s="310"/>
     </row>
     <row r="16" spans="2:10" s="115" customFormat="1" ht="15.6" customHeight="1">
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="292"/>
-      <c r="E16" s="277" t="s">
+      <c r="B16" s="293"/>
+      <c r="C16" s="293"/>
+      <c r="D16" s="325"/>
+      <c r="E16" s="310" t="s">
         <v>465</v>
       </c>
-      <c r="F16" s="277"/>
-      <c r="G16" s="277"/>
-      <c r="H16" s="277"/>
-      <c r="I16" s="277"/>
-      <c r="J16" s="277"/>
+      <c r="F16" s="310"/>
+      <c r="G16" s="310"/>
+      <c r="H16" s="310"/>
+      <c r="I16" s="310"/>
+      <c r="J16" s="310"/>
     </row>
     <row r="17" spans="1:10" s="115" customFormat="1" ht="41.45" customHeight="1">
-      <c r="B17" s="260"/>
-      <c r="C17" s="260"/>
-      <c r="D17" s="292"/>
-      <c r="E17" s="293" t="s">
+      <c r="B17" s="293"/>
+      <c r="C17" s="293"/>
+      <c r="D17" s="325"/>
+      <c r="E17" s="326" t="s">
         <v>570</v>
       </c>
-      <c r="F17" s="294"/>
-      <c r="G17" s="265" t="s">
+      <c r="F17" s="327"/>
+      <c r="G17" s="298" t="s">
         <v>457</v>
       </c>
-      <c r="H17" s="265"/>
-      <c r="I17" s="265"/>
-      <c r="J17" s="265"/>
+      <c r="H17" s="298"/>
+      <c r="I17" s="298"/>
+      <c r="J17" s="298"/>
     </row>
     <row r="18" spans="1:10" s="115" customFormat="1" ht="24" customHeight="1">
       <c r="B18" s="207"/>
       <c r="C18" s="207"/>
       <c r="D18" s="116"/>
-      <c r="E18" s="261" t="s">
+      <c r="E18" s="294" t="s">
         <v>459</v>
       </c>
-      <c r="F18" s="261"/>
-      <c r="G18" s="261"/>
-      <c r="H18" s="261"/>
-      <c r="I18" s="261"/>
-      <c r="J18" s="261"/>
+      <c r="F18" s="294"/>
+      <c r="G18" s="294"/>
+      <c r="H18" s="294"/>
+      <c r="I18" s="294"/>
+      <c r="J18" s="294"/>
     </row>
     <row r="19" spans="1:10" s="115" customFormat="1" ht="30" customHeight="1">
       <c r="B19" s="208" t="s">
@@ -13097,14 +13207,14 @@
       <c r="D19" s="119">
         <v>4</v>
       </c>
-      <c r="E19" s="277" t="s">
+      <c r="E19" s="310" t="s">
         <v>463</v>
       </c>
-      <c r="F19" s="277"/>
-      <c r="G19" s="277"/>
-      <c r="H19" s="277"/>
-      <c r="I19" s="277"/>
-      <c r="J19" s="277"/>
+      <c r="F19" s="310"/>
+      <c r="G19" s="310"/>
+      <c r="H19" s="310"/>
+      <c r="I19" s="310"/>
+      <c r="J19" s="310"/>
     </row>
     <row r="20" spans="1:10" s="115" customFormat="1" ht="22.5" customHeight="1">
       <c r="A20" s="40"/>
@@ -13124,15 +13234,15 @@
       <c r="B21" s="40" t="s">
         <v>455</v>
       </c>
-      <c r="C21" s="290" t="s">
+      <c r="C21" s="323" t="s">
         <v>456</v>
       </c>
-      <c r="D21" s="290"/>
-      <c r="E21" s="290"/>
-      <c r="H21" s="264" t="s">
+      <c r="D21" s="323"/>
+      <c r="E21" s="323"/>
+      <c r="H21" s="297" t="s">
         <v>565</v>
       </c>
-      <c r="I21" s="264"/>
+      <c r="I21" s="297"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="C22" s="40" t="s">
@@ -13143,10 +13253,10 @@
       </c>
       <c r="F22" s="85"/>
       <c r="G22" s="85"/>
-      <c r="H22" s="264" t="s">
+      <c r="H22" s="297" t="s">
         <v>562</v>
       </c>
-      <c r="I22" s="264"/>
+      <c r="I22" s="297"/>
       <c r="J22" s="85"/>
     </row>
     <row r="23" spans="1:10" ht="14.1" customHeight="1">
@@ -13154,15 +13264,15 @@
         <v>448</v>
       </c>
       <c r="D23" s="118"/>
-      <c r="E23" s="289" t="s">
+      <c r="E23" s="322" t="s">
         <v>452</v>
       </c>
-      <c r="F23" s="289"/>
+      <c r="F23" s="322"/>
       <c r="G23" s="85"/>
-      <c r="H23" s="287" t="s">
+      <c r="H23" s="320" t="s">
         <v>443</v>
       </c>
-      <c r="I23" s="287"/>
+      <c r="I23" s="320"/>
       <c r="J23" s="85"/>
     </row>
     <row r="24" spans="1:10">
@@ -13174,10 +13284,10 @@
       </c>
       <c r="F24" s="85"/>
       <c r="G24" s="85"/>
-      <c r="H24" s="264" t="s">
+      <c r="H24" s="297" t="s">
         <v>442</v>
       </c>
-      <c r="I24" s="264"/>
+      <c r="I24" s="297"/>
       <c r="J24" s="85"/>
     </row>
     <row r="25" spans="1:10">
@@ -13189,30 +13299,30 @@
       </c>
       <c r="F25" s="85"/>
       <c r="G25" s="85"/>
-      <c r="H25" s="265" t="s">
+      <c r="H25" s="298" t="s">
         <v>444</v>
       </c>
-      <c r="I25" s="265"/>
+      <c r="I25" s="298"/>
       <c r="J25" s="85"/>
     </row>
     <row r="26" spans="1:10">
       <c r="E26" s="85"/>
       <c r="F26" s="85"/>
       <c r="G26" s="85"/>
-      <c r="H26" s="287" t="s">
+      <c r="H26" s="320" t="s">
         <v>563</v>
       </c>
-      <c r="I26" s="287"/>
+      <c r="I26" s="320"/>
       <c r="J26" s="85"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="E27" s="85"/>
       <c r="F27" s="85"/>
       <c r="G27" s="85"/>
-      <c r="H27" s="287" t="s">
+      <c r="H27" s="320" t="s">
         <v>564</v>
       </c>
-      <c r="I27" s="287"/>
+      <c r="I27" s="320"/>
       <c r="J27" s="85"/>
     </row>
     <row r="28" spans="1:10">
@@ -13420,11 +13530,11 @@
       <c r="B3" s="41"/>
       <c r="C3" s="42"/>
       <c r="D3" s="45"/>
-      <c r="E3" s="296" t="s">
+      <c r="E3" s="329" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="297"/>
-      <c r="G3" s="298"/>
+      <c r="F3" s="330"/>
+      <c r="G3" s="331"/>
       <c r="H3" s="45"/>
       <c r="I3" s="45"/>
     </row>
@@ -13469,14 +13579,14 @@
     <row r="6" spans="2:9" ht="12.75" thickBot="1">
       <c r="B6" s="41"/>
       <c r="C6" s="42"/>
-      <c r="D6" s="299" t="s">
+      <c r="D6" s="332" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="300"/>
-      <c r="F6" s="300"/>
-      <c r="G6" s="300"/>
-      <c r="H6" s="300"/>
-      <c r="I6" s="301"/>
+      <c r="E6" s="333"/>
+      <c r="F6" s="333"/>
+      <c r="G6" s="333"/>
+      <c r="H6" s="333"/>
+      <c r="I6" s="334"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" thickBot="1">
       <c r="B7" s="41"/>
@@ -13525,34 +13635,34 @@
     <row r="9" spans="2:9" ht="12.75" thickBot="1">
       <c r="B9" s="41"/>
       <c r="C9" s="42"/>
-      <c r="D9" s="302" t="s">
+      <c r="D9" s="335" t="s">
         <v>269</v>
       </c>
-      <c r="E9" s="303"/>
-      <c r="F9" s="303"/>
-      <c r="G9" s="303"/>
-      <c r="H9" s="303"/>
-      <c r="I9" s="304"/>
+      <c r="E9" s="336"/>
+      <c r="F9" s="336"/>
+      <c r="G9" s="336"/>
+      <c r="H9" s="336"/>
+      <c r="I9" s="337"/>
     </row>
     <row r="10" spans="2:9" ht="12.75" thickBot="1">
       <c r="B10" s="41"/>
       <c r="C10" s="42"/>
-      <c r="D10" s="305"/>
-      <c r="E10" s="306"/>
-      <c r="F10" s="306"/>
-      <c r="G10" s="306"/>
-      <c r="H10" s="306"/>
-      <c r="I10" s="307"/>
+      <c r="D10" s="338"/>
+      <c r="E10" s="339"/>
+      <c r="F10" s="339"/>
+      <c r="G10" s="339"/>
+      <c r="H10" s="339"/>
+      <c r="I10" s="340"/>
     </row>
     <row r="11" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B11" s="310" t="s">
+      <c r="B11" s="343" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="55"/>
-      <c r="D11" s="308" t="s">
+      <c r="D11" s="341" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="309"/>
+      <c r="E11" s="342"/>
       <c r="F11" s="56" t="s">
         <v>5</v>
       </c>
@@ -13567,7 +13677,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B12" s="311"/>
+      <c r="B12" s="344"/>
       <c r="C12" s="80"/>
       <c r="D12" s="81"/>
       <c r="E12" s="81"/>
@@ -13581,10 +13691,10 @@
       <c r="C13" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="312" t="s">
+      <c r="D13" s="345" t="s">
         <v>534</v>
       </c>
-      <c r="E13" s="313"/>
+      <c r="E13" s="346"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -13595,46 +13705,46 @@
       <c r="C14" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="323" t="s">
+      <c r="D14" s="356" t="s">
         <v>772</v>
       </c>
-      <c r="E14" s="324"/>
-      <c r="F14" s="324"/>
-      <c r="G14" s="324"/>
-      <c r="H14" s="324"/>
-      <c r="I14" s="325"/>
+      <c r="E14" s="357"/>
+      <c r="F14" s="357"/>
+      <c r="G14" s="357"/>
+      <c r="H14" s="357"/>
+      <c r="I14" s="358"/>
     </row>
     <row r="15" spans="2:9" ht="14.45" customHeight="1">
-      <c r="B15" s="310" t="s">
+      <c r="B15" s="343" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="310"/>
-      <c r="D15" s="315" t="s">
+      <c r="C15" s="343"/>
+      <c r="D15" s="348" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="316"/>
-      <c r="F15" s="316"/>
-      <c r="G15" s="316"/>
-      <c r="H15" s="316"/>
-      <c r="I15" s="317"/>
+      <c r="E15" s="349"/>
+      <c r="F15" s="349"/>
+      <c r="G15" s="349"/>
+      <c r="H15" s="349"/>
+      <c r="I15" s="350"/>
     </row>
     <row r="16" spans="2:9" ht="12.75" thickBot="1">
-      <c r="B16" s="311"/>
-      <c r="C16" s="311"/>
-      <c r="D16" s="318"/>
-      <c r="E16" s="319"/>
-      <c r="F16" s="319"/>
-      <c r="G16" s="319"/>
-      <c r="H16" s="319"/>
-      <c r="I16" s="320"/>
+      <c r="B16" s="344"/>
+      <c r="C16" s="344"/>
+      <c r="D16" s="351"/>
+      <c r="E16" s="352"/>
+      <c r="F16" s="352"/>
+      <c r="G16" s="352"/>
+      <c r="H16" s="352"/>
+      <c r="I16" s="353"/>
     </row>
     <row r="17" spans="2:9" ht="12.75" thickBot="1">
-      <c r="B17" s="311"/>
-      <c r="C17" s="311"/>
-      <c r="D17" s="308" t="s">
+      <c r="B17" s="344"/>
+      <c r="C17" s="344"/>
+      <c r="D17" s="341" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="309"/>
+      <c r="E17" s="342"/>
       <c r="F17" s="56" t="s">
         <v>5</v>
       </c>
@@ -13649,12 +13759,12 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="12.75" thickBot="1">
-      <c r="B18" s="314"/>
-      <c r="C18" s="314"/>
-      <c r="D18" s="321" t="s">
+      <c r="B18" s="347"/>
+      <c r="C18" s="347"/>
+      <c r="D18" s="354" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="322"/>
+      <c r="E18" s="355"/>
       <c r="F18" s="62"/>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
@@ -13663,10 +13773,10 @@
     <row r="19" spans="2:9" ht="15" customHeight="1" thickBot="1">
       <c r="B19" s="64"/>
       <c r="C19" s="64"/>
-      <c r="D19" s="308" t="s">
+      <c r="D19" s="341" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="309"/>
+      <c r="E19" s="342"/>
       <c r="F19" s="56" t="s">
         <v>5</v>
       </c>
@@ -13681,58 +13791,58 @@
       </c>
     </row>
     <row r="20" spans="2:9" ht="36.6" customHeight="1" thickBot="1">
-      <c r="B20" s="310" t="s">
+      <c r="B20" s="343" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="64"/>
-      <c r="D20" s="312" t="s">
+      <c r="D20" s="345" t="s">
         <v>535</v>
       </c>
-      <c r="E20" s="326"/>
-      <c r="F20" s="326"/>
-      <c r="G20" s="326"/>
-      <c r="H20" s="326"/>
-      <c r="I20" s="327"/>
+      <c r="E20" s="359"/>
+      <c r="F20" s="359"/>
+      <c r="G20" s="359"/>
+      <c r="H20" s="359"/>
+      <c r="I20" s="360"/>
     </row>
     <row r="21" spans="2:9" ht="103.5" customHeight="1" thickBot="1">
-      <c r="B21" s="311"/>
+      <c r="B21" s="344"/>
       <c r="C21" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="312" t="s">
+      <c r="D21" s="345" t="s">
         <v>771</v>
       </c>
-      <c r="E21" s="326"/>
-      <c r="F21" s="326"/>
-      <c r="G21" s="326"/>
-      <c r="H21" s="326"/>
-      <c r="I21" s="313"/>
+      <c r="E21" s="359"/>
+      <c r="F21" s="359"/>
+      <c r="G21" s="359"/>
+      <c r="H21" s="359"/>
+      <c r="I21" s="346"/>
     </row>
     <row r="22" spans="2:9" ht="135" customHeight="1" thickBot="1">
-      <c r="B22" s="314"/>
+      <c r="B22" s="347"/>
       <c r="C22" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="323" t="s">
+      <c r="D22" s="356" t="s">
         <v>774</v>
       </c>
-      <c r="E22" s="324"/>
-      <c r="F22" s="324"/>
-      <c r="G22" s="324"/>
-      <c r="H22" s="324"/>
-      <c r="I22" s="325"/>
+      <c r="E22" s="357"/>
+      <c r="F22" s="357"/>
+      <c r="G22" s="357"/>
+      <c r="H22" s="357"/>
+      <c r="I22" s="358"/>
     </row>
     <row r="23" spans="2:9" ht="12.75" thickBot="1">
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
       <c r="D23" s="66"/>
-      <c r="E23" s="331" t="s">
+      <c r="E23" s="364" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="332"/>
-      <c r="G23" s="332"/>
-      <c r="H23" s="332"/>
-      <c r="I23" s="333"/>
+      <c r="F23" s="365"/>
+      <c r="G23" s="365"/>
+      <c r="H23" s="365"/>
+      <c r="I23" s="366"/>
     </row>
     <row r="24" spans="2:9" ht="12.75" thickBot="1">
       <c r="B24" s="67"/>
@@ -13755,10 +13865,10 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B25" s="334" t="s">
+      <c r="B25" s="367" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="334" t="s">
+      <c r="C25" s="367" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="73"/>
@@ -13779,8 +13889,8 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="96.75" thickBot="1">
-      <c r="B26" s="335"/>
-      <c r="C26" s="335"/>
+      <c r="B26" s="368"/>
+      <c r="C26" s="368"/>
       <c r="D26" s="61" t="s">
         <v>6</v>
       </c>
@@ -13801,8 +13911,8 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B27" s="335"/>
-      <c r="C27" s="335"/>
+      <c r="B27" s="368"/>
+      <c r="C27" s="368"/>
       <c r="D27" s="73" t="s">
         <v>19</v>
       </c>
@@ -13813,8 +13923,8 @@
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="2:9" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B28" s="335"/>
-      <c r="C28" s="335"/>
+      <c r="B28" s="368"/>
+      <c r="C28" s="368"/>
       <c r="D28" s="73" t="s">
         <v>21</v>
       </c>
@@ -13825,8 +13935,8 @@
       <c r="I28" s="12"/>
     </row>
     <row r="29" spans="2:9" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B29" s="335"/>
-      <c r="C29" s="335"/>
+      <c r="B29" s="368"/>
+      <c r="C29" s="368"/>
       <c r="D29" s="73" t="s">
         <v>20</v>
       </c>
@@ -13837,8 +13947,8 @@
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="2:9" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B30" s="336"/>
-      <c r="C30" s="336"/>
+      <c r="B30" s="369"/>
+      <c r="C30" s="369"/>
       <c r="D30" s="74" t="s">
         <v>22</v>
       </c>
@@ -13849,30 +13959,30 @@
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B31" s="310" t="s">
+      <c r="B31" s="343" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="75"/>
-      <c r="D31" s="340" t="s">
+      <c r="D31" s="373" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="341"/>
-      <c r="F31" s="341"/>
-      <c r="G31" s="341"/>
-      <c r="H31" s="341"/>
-      <c r="I31" s="342"/>
+      <c r="E31" s="374"/>
+      <c r="F31" s="374"/>
+      <c r="G31" s="374"/>
+      <c r="H31" s="374"/>
+      <c r="I31" s="375"/>
     </row>
     <row r="32" spans="2:9" ht="12.75" thickBot="1">
-      <c r="B32" s="311"/>
+      <c r="B32" s="344"/>
       <c r="C32" s="76"/>
-      <c r="D32" s="343" t="s">
+      <c r="D32" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="344"/>
-      <c r="F32" s="343" t="s">
+      <c r="E32" s="377"/>
+      <c r="F32" s="376" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="345"/>
+      <c r="G32" s="378"/>
       <c r="H32" s="70" t="s">
         <v>18</v>
       </c>
@@ -13881,64 +13991,64 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="77.45" customHeight="1" thickBot="1">
-      <c r="B33" s="311"/>
+      <c r="B33" s="344"/>
       <c r="C33" s="245" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="329" t="s">
+      <c r="D33" s="362" t="s">
         <v>773</v>
       </c>
-      <c r="E33" s="330"/>
-      <c r="F33" s="330"/>
-      <c r="G33" s="330"/>
-      <c r="H33" s="330"/>
-      <c r="I33" s="330"/>
+      <c r="E33" s="363"/>
+      <c r="F33" s="363"/>
+      <c r="G33" s="363"/>
+      <c r="H33" s="363"/>
+      <c r="I33" s="363"/>
     </row>
     <row r="34" spans="2:9" ht="63.95" customHeight="1" thickBot="1">
-      <c r="B34" s="337"/>
+      <c r="B34" s="370"/>
       <c r="C34" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="312" t="s">
+      <c r="D34" s="345" t="s">
         <v>924</v>
       </c>
-      <c r="E34" s="326"/>
-      <c r="F34" s="326"/>
-      <c r="G34" s="326"/>
-      <c r="H34" s="326"/>
-      <c r="I34" s="313"/>
+      <c r="E34" s="359"/>
+      <c r="F34" s="359"/>
+      <c r="G34" s="359"/>
+      <c r="H34" s="359"/>
+      <c r="I34" s="346"/>
     </row>
     <row r="35" spans="2:9" ht="120.6" customHeight="1" thickBot="1">
-      <c r="B35" s="338"/>
+      <c r="B35" s="371"/>
       <c r="C35" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="323" t="s">
+      <c r="D35" s="356" t="s">
         <v>537</v>
       </c>
-      <c r="E35" s="324"/>
-      <c r="F35" s="324"/>
-      <c r="G35" s="324"/>
-      <c r="H35" s="324"/>
-      <c r="I35" s="328"/>
+      <c r="E35" s="357"/>
+      <c r="F35" s="357"/>
+      <c r="G35" s="357"/>
+      <c r="H35" s="357"/>
+      <c r="I35" s="361"/>
     </row>
     <row r="36" spans="2:9" ht="12.75" thickBot="1">
-      <c r="B36" s="338"/>
+      <c r="B36" s="371"/>
       <c r="C36" s="61"/>
-      <c r="D36" s="312" t="s">
+      <c r="D36" s="345" t="s">
         <v>536</v>
       </c>
-      <c r="E36" s="313"/>
+      <c r="E36" s="346"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="2:9" ht="12.75" thickBot="1">
-      <c r="B37" s="339"/>
+      <c r="B37" s="372"/>
       <c r="C37" s="61"/>
-      <c r="D37" s="323"/>
-      <c r="E37" s="325"/>
+      <c r="D37" s="356"/>
+      <c r="E37" s="358"/>
       <c r="F37" s="39"/>
       <c r="G37" s="39"/>
       <c r="H37" s="39"/>
@@ -14006,9 +14116,9 @@
     <col min="6" max="6" width="38.85546875" customWidth="1"/>
     <col min="7" max="7" width="36.5703125" customWidth="1"/>
     <col min="8" max="8" width="43.140625" customWidth="1"/>
-    <col min="10" max="10" width="46.140625" style="436" customWidth="1"/>
-    <col min="11" max="11" width="58" style="436" customWidth="1"/>
-    <col min="12" max="12" width="63.42578125" style="436" customWidth="1"/>
+    <col min="10" max="10" width="46.140625" style="254" customWidth="1"/>
+    <col min="11" max="11" width="58" style="254" customWidth="1"/>
+    <col min="12" max="12" width="63.42578125" style="254" customWidth="1"/>
     <col min="13" max="13" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14022,18 +14132,18 @@
       <c r="H2" s="3"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1">
-      <c r="L4" s="441"/>
+      <c r="L4" s="259"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C5" s="346" t="s">
+      <c r="C5" s="379" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="347"/>
-      <c r="E5" s="347"/>
-      <c r="F5" s="347"/>
-      <c r="G5" s="347"/>
-      <c r="H5" s="348"/>
-      <c r="K5" s="439"/>
+      <c r="D5" s="380"/>
+      <c r="E5" s="380"/>
+      <c r="F5" s="380"/>
+      <c r="G5" s="380"/>
+      <c r="H5" s="381"/>
+      <c r="K5" s="257"/>
     </row>
     <row r="6" spans="2:12" ht="36.75" thickBot="1">
       <c r="B6" s="27" t="s">
@@ -14059,7 +14169,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="24">
-      <c r="B7" s="349" t="s">
+      <c r="B7" s="382" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="28"/>
@@ -14067,7 +14177,7 @@
       <c r="E7" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="F7" s="452" t="s">
+      <c r="F7" s="270" t="s">
         <v>334</v>
       </c>
       <c r="G7" s="30" t="s">
@@ -14078,13 +14188,13 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="24">
-      <c r="B8" s="350"/>
+      <c r="B8" s="383"/>
       <c r="C8" s="32"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="F8" s="451" t="s">
+      <c r="F8" s="269" t="s">
         <v>335</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -14095,7 +14205,7 @@
       </c>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="350"/>
+      <c r="B9" s="383"/>
       <c r="C9" s="32"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16" t="s">
@@ -14112,13 +14222,13 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="24">
-      <c r="B10" s="350"/>
+      <c r="B10" s="383"/>
       <c r="C10" s="32"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="F10" s="451" t="s">
+      <c r="F10" s="269" t="s">
         <v>337</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -14129,7 +14239,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="24">
-      <c r="B11" s="350"/>
+      <c r="B11" s="383"/>
       <c r="C11" s="32"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
@@ -14144,7 +14254,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B12" s="351"/>
+      <c r="B12" s="384"/>
       <c r="C12" s="33"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17" t="s">
@@ -14157,7 +14267,7 @@
       <c r="H12" s="23"/>
     </row>
     <row r="13" spans="2:12" ht="36">
-      <c r="B13" s="349" t="s">
+      <c r="B13" s="382" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="28"/>
@@ -14176,7 +14286,7 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="24">
-      <c r="B14" s="350"/>
+      <c r="B14" s="383"/>
       <c r="C14" s="32"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16" t="s">
@@ -14193,7 +14303,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="36">
-      <c r="B15" s="350"/>
+      <c r="B15" s="383"/>
       <c r="C15" s="32"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
@@ -14208,7 +14318,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="24.75" thickBot="1">
-      <c r="B16" s="350"/>
+      <c r="B16" s="383"/>
       <c r="C16" s="33"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17" t="s">
@@ -14223,7 +14333,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="36.75" thickBot="1">
-      <c r="B17" s="351"/>
+      <c r="B17" s="384"/>
       <c r="C17" s="33"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17" t="s">
@@ -14236,7 +14346,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="60">
-      <c r="B18" s="349" t="s">
+      <c r="B18" s="382" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="25"/>
@@ -14255,7 +14365,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="36">
-      <c r="B19" s="350"/>
+      <c r="B19" s="383"/>
       <c r="C19" s="25"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16" t="s">
@@ -14272,7 +14382,7 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="48.75" thickBot="1">
-      <c r="B20" s="351"/>
+      <c r="B20" s="384"/>
       <c r="C20" s="26"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19" t="s">
@@ -14289,7 +14399,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="36">
-      <c r="B21" s="349" t="s">
+      <c r="B21" s="382" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="28"/>
@@ -14308,7 +14418,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="24">
-      <c r="B22" s="350"/>
+      <c r="B22" s="383"/>
       <c r="C22" s="32"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16" t="s">
@@ -14325,7 +14435,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="24">
-      <c r="B23" s="350"/>
+      <c r="B23" s="383"/>
       <c r="C23" s="32"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16" t="s">
@@ -14342,7 +14452,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="24">
-      <c r="B24" s="350"/>
+      <c r="B24" s="383"/>
       <c r="C24" s="32"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16" t="s">
@@ -14357,7 +14467,7 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="48">
-      <c r="B25" s="350"/>
+      <c r="B25" s="383"/>
       <c r="C25" s="32"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
@@ -14370,7 +14480,7 @@
       <c r="H25" s="18"/>
     </row>
     <row r="26" spans="2:8" ht="24.75" thickBot="1">
-      <c r="B26" s="351"/>
+      <c r="B26" s="384"/>
       <c r="C26" s="33"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17" t="s">
@@ -14383,7 +14493,7 @@
       <c r="H26" s="23"/>
     </row>
     <row r="27" spans="2:8" ht="36">
-      <c r="B27" s="349" t="s">
+      <c r="B27" s="382" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="28"/>
@@ -14402,7 +14512,7 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="36">
-      <c r="B28" s="350"/>
+      <c r="B28" s="383"/>
       <c r="C28" s="32"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16" t="s">
@@ -14419,7 +14529,7 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="48">
-      <c r="B29" s="350"/>
+      <c r="B29" s="383"/>
       <c r="C29" s="32"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16" t="s">
@@ -14436,7 +14546,7 @@
       </c>
     </row>
     <row r="30" spans="2:8" ht="24">
-      <c r="B30" s="350"/>
+      <c r="B30" s="383"/>
       <c r="C30" s="32"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16" t="s">
@@ -14453,7 +14563,7 @@
       </c>
     </row>
     <row r="31" spans="2:8" ht="48">
-      <c r="B31" s="350"/>
+      <c r="B31" s="383"/>
       <c r="C31" s="32"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16" t="s">
@@ -14470,7 +14580,7 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="60.75" thickBot="1">
-      <c r="B32" s="351"/>
+      <c r="B32" s="384"/>
       <c r="C32" s="33"/>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
@@ -14485,7 +14595,7 @@
       <c r="H32" s="23"/>
     </row>
     <row r="33" spans="2:8" ht="36">
-      <c r="B33" s="349" t="s">
+      <c r="B33" s="382" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="28"/>
@@ -14504,7 +14614,7 @@
       </c>
     </row>
     <row r="34" spans="2:8" ht="60">
-      <c r="B34" s="350"/>
+      <c r="B34" s="383"/>
       <c r="C34" s="32"/>
       <c r="D34" s="16"/>
       <c r="E34" s="16" t="s">
@@ -14521,7 +14631,7 @@
       </c>
     </row>
     <row r="35" spans="2:8" ht="48">
-      <c r="B35" s="350"/>
+      <c r="B35" s="383"/>
       <c r="C35" s="32"/>
       <c r="D35" s="16"/>
       <c r="E35" s="16" t="s">
@@ -14538,7 +14648,7 @@
       </c>
     </row>
     <row r="36" spans="2:8" ht="24">
-      <c r="B36" s="350"/>
+      <c r="B36" s="383"/>
       <c r="C36" s="32"/>
       <c r="D36" s="16"/>
       <c r="E36" s="16" t="s">
@@ -14553,7 +14663,7 @@
       </c>
     </row>
     <row r="37" spans="2:8" ht="24.75" thickBot="1">
-      <c r="B37" s="351"/>
+      <c r="B37" s="384"/>
       <c r="C37" s="33"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17" t="s">
@@ -14566,7 +14676,7 @@
       <c r="H37" s="23"/>
     </row>
     <row r="38" spans="2:8" ht="36">
-      <c r="B38" s="349" t="s">
+      <c r="B38" s="382" t="s">
         <v>102</v>
       </c>
       <c r="C38" s="28"/>
@@ -14585,7 +14695,7 @@
       </c>
     </row>
     <row r="39" spans="2:8" ht="48">
-      <c r="B39" s="350"/>
+      <c r="B39" s="383"/>
       <c r="C39" s="32"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16" t="s">
@@ -14602,7 +14712,7 @@
       </c>
     </row>
     <row r="40" spans="2:8" ht="36">
-      <c r="B40" s="350"/>
+      <c r="B40" s="383"/>
       <c r="C40" s="32"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16" t="s">
@@ -14619,7 +14729,7 @@
       </c>
     </row>
     <row r="41" spans="2:8" ht="24">
-      <c r="B41" s="350"/>
+      <c r="B41" s="383"/>
       <c r="C41" s="32"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16" t="s">
@@ -14634,7 +14744,7 @@
       </c>
     </row>
     <row r="42" spans="2:8" ht="24.75" thickBot="1">
-      <c r="B42" s="351"/>
+      <c r="B42" s="384"/>
       <c r="C42" s="33"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17" t="s">
@@ -14647,7 +14757,7 @@
       </c>
     </row>
     <row r="43" spans="2:8" ht="36">
-      <c r="B43" s="349" t="s">
+      <c r="B43" s="382" t="s">
         <v>56</v>
       </c>
       <c r="C43" s="28"/>
@@ -14666,7 +14776,7 @@
       </c>
     </row>
     <row r="44" spans="2:8" ht="48">
-      <c r="B44" s="350"/>
+      <c r="B44" s="383"/>
       <c r="C44" s="32"/>
       <c r="D44" s="16"/>
       <c r="E44" s="16" t="s">
@@ -14683,7 +14793,7 @@
       </c>
     </row>
     <row r="45" spans="2:8" ht="36">
-      <c r="B45" s="350"/>
+      <c r="B45" s="383"/>
       <c r="C45" s="32"/>
       <c r="D45" s="16"/>
       <c r="E45" s="16" t="s">
@@ -14700,7 +14810,7 @@
       </c>
     </row>
     <row r="46" spans="2:8" ht="36">
-      <c r="B46" s="350"/>
+      <c r="B46" s="383"/>
       <c r="C46" s="32"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16" t="s">
@@ -14715,7 +14825,7 @@
       </c>
     </row>
     <row r="47" spans="2:8" ht="24.75" thickBot="1">
-      <c r="B47" s="351"/>
+      <c r="B47" s="384"/>
       <c r="C47" s="33"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17" t="s">
@@ -14750,7 +14860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F9D293-EABB-44FD-8A3A-A054B35416AB}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -14762,54 +14872,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5">
-      <c r="A1" s="438" t="s">
+      <c r="A1" s="256" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="440" t="s">
+      <c r="B1" s="258" t="s">
         <v>928</v>
       </c>
-      <c r="C1" s="440" t="s">
+      <c r="C1" s="258" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75">
-      <c r="A2" s="435" t="s">
+      <c r="A2" s="253" t="s">
         <v>927</v>
       </c>
-      <c r="B2" s="437" t="s">
+      <c r="B2" s="255" t="s">
         <v>929</v>
       </c>
-      <c r="C2" s="442" t="s">
+      <c r="C2" s="260" t="s">
         <v>933</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="300">
-      <c r="A3" s="443" t="s">
+      <c r="A3" s="261" t="s">
         <v>930</v>
       </c>
-      <c r="B3" s="444" t="s">
+      <c r="B3" s="262" t="s">
         <v>931</v>
       </c>
-      <c r="C3" s="443" t="s">
+      <c r="C3" s="261" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="135">
-      <c r="A4" s="445" t="s">
+      <c r="A4" s="263" t="s">
         <v>932</v>
       </c>
-      <c r="B4" s="446" t="s">
+      <c r="B4" s="264" t="s">
         <v>934</v>
       </c>
-      <c r="C4" s="447" t="s">
+      <c r="C4" s="265" t="s">
         <v>935</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="90">
-      <c r="A5" s="443" t="s">
+      <c r="A5" s="261" t="s">
         <v>936</v>
       </c>
-      <c r="B5" s="448" t="s">
+      <c r="B5" s="266" t="s">
         <v>937</v>
       </c>
       <c r="C5" s="252" t="s">
@@ -14817,10 +14927,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="90">
-      <c r="A6" s="443" t="s">
+      <c r="A6" s="261" t="s">
         <v>940</v>
       </c>
-      <c r="B6" s="449" t="s">
+      <c r="B6" s="267" t="s">
         <v>941</v>
       </c>
       <c r="C6" s="252" t="s">
@@ -14828,10 +14938,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="75">
-      <c r="A7" s="445" t="s">
+      <c r="A7" s="263" t="s">
         <v>943</v>
       </c>
-      <c r="B7" s="450" t="s">
+      <c r="B7" s="268" t="s">
         <v>925</v>
       </c>
       <c r="C7" s="252" t="s">
@@ -14839,32 +14949,32 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="75">
-      <c r="A8" s="445" t="s">
+      <c r="A8" s="263" t="s">
         <v>946</v>
       </c>
-      <c r="B8" s="437" t="s">
+      <c r="B8" s="255" t="s">
         <v>929</v>
       </c>
-      <c r="C8" s="443" t="s">
+      <c r="C8" s="261" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60">
-      <c r="A9" s="443" t="s">
+      <c r="A9" s="261" t="s">
         <v>947</v>
       </c>
-      <c r="B9" s="446" t="s">
+      <c r="B9" s="264" t="s">
         <v>934</v>
       </c>
-      <c r="C9" s="453" t="s">
+      <c r="C9" s="271" t="s">
         <v>948</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="90">
-      <c r="A10" s="443" t="s">
+      <c r="A10" s="261" t="s">
         <v>949</v>
       </c>
-      <c r="B10" s="448" t="s">
+      <c r="B10" s="266" t="s">
         <v>937</v>
       </c>
       <c r="C10" s="252" t="s">
@@ -14872,35 +14982,35 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="60">
-      <c r="A11" s="443" t="s">
+      <c r="A11" s="261" t="s">
         <v>950</v>
       </c>
-      <c r="B11" s="455" t="s">
+      <c r="B11" s="273" t="s">
         <v>952</v>
       </c>
-      <c r="C11" s="454" t="s">
+      <c r="C11" s="272" t="s">
         <v>951</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="75">
-      <c r="A12" s="445" t="s">
+      <c r="A12" s="263" t="s">
         <v>953</v>
       </c>
-      <c r="B12" s="444" t="s">
+      <c r="B12" s="262" t="s">
         <v>931</v>
       </c>
-      <c r="C12" s="453" t="s">
+      <c r="C12" s="271" t="s">
         <v>954</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="75">
-      <c r="A13" s="457" t="s">
+      <c r="A13" s="275" t="s">
         <v>955</v>
       </c>
-      <c r="B13" s="458" t="s">
+      <c r="B13" s="276" t="s">
         <v>929</v>
       </c>
-      <c r="C13" s="456" t="s">
+      <c r="C13" s="274" t="s">
         <v>956</v>
       </c>
     </row>
@@ -14908,10 +15018,10 @@
       <c r="A14" s="252" t="s">
         <v>957</v>
       </c>
-      <c r="B14" s="448" t="s">
+      <c r="B14" s="266" t="s">
         <v>937</v>
       </c>
-      <c r="C14" s="453" t="s">
+      <c r="C14" s="271" t="s">
         <v>958</v>
       </c>
     </row>
@@ -14919,10 +15029,10 @@
       <c r="A15" s="252" t="s">
         <v>959</v>
       </c>
-      <c r="B15" s="446" t="s">
+      <c r="B15" s="264" t="s">
         <v>934</v>
       </c>
-      <c r="C15" s="453" t="s">
+      <c r="C15" s="271" t="s">
         <v>960</v>
       </c>
     </row>
@@ -14930,29 +15040,29 @@
       <c r="A16" s="252" t="s">
         <v>961</v>
       </c>
-      <c r="B16" s="455" t="s">
+      <c r="B16" s="273" t="s">
         <v>952</v>
       </c>
-      <c r="C16" s="453" t="s">
+      <c r="C16" s="271" t="s">
         <v>962</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="60">
-      <c r="A17" s="443" t="s">
+      <c r="A17" s="261" t="s">
         <v>963</v>
       </c>
-      <c r="B17" s="446" t="s">
+      <c r="B17" s="264" t="s">
         <v>934</v>
       </c>
-      <c r="C17" s="453" t="s">
+      <c r="C17" s="271" t="s">
         <v>964</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60">
-      <c r="A18" s="443" t="s">
+      <c r="A18" s="261" t="s">
         <v>965</v>
       </c>
-      <c r="B18" s="450" t="s">
+      <c r="B18" s="268" t="s">
         <v>925</v>
       </c>
       <c r="C18" s="252" t="s">
@@ -14960,10 +15070,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="60">
-      <c r="A19" s="443" t="s">
+      <c r="A19" s="261" t="s">
         <v>967</v>
       </c>
-      <c r="B19" s="437" t="s">
+      <c r="B19" s="255" t="s">
         <v>929</v>
       </c>
       <c r="C19" s="252" t="s">
@@ -14971,43 +15081,43 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="60">
-      <c r="A20" s="443" t="s">
+      <c r="A20" s="261" t="s">
         <v>969</v>
       </c>
-      <c r="B20" s="444" t="s">
+      <c r="B20" s="262" t="s">
         <v>931</v>
       </c>
-      <c r="C20" s="453" t="s">
+      <c r="C20" s="271" t="s">
         <v>970</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="60">
-      <c r="A21" s="443" t="s">
+      <c r="A21" s="261" t="s">
         <v>971</v>
       </c>
-      <c r="B21" s="437" t="s">
+      <c r="B21" s="255" t="s">
         <v>929</v>
       </c>
-      <c r="C21" s="453" t="s">
+      <c r="C21" s="271" t="s">
         <v>978</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="60">
-      <c r="A22" s="443" t="s">
+      <c r="A22" s="261" t="s">
         <v>972</v>
       </c>
-      <c r="B22" s="455" t="s">
+      <c r="B22" s="273" t="s">
         <v>952</v>
       </c>
-      <c r="C22" s="453" t="s">
+      <c r="C22" s="271" t="s">
         <v>979</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="75">
-      <c r="A23" s="443" t="s">
+      <c r="A23" s="261" t="s">
         <v>973</v>
       </c>
-      <c r="B23" s="444" t="s">
+      <c r="B23" s="262" t="s">
         <v>931</v>
       </c>
       <c r="C23" s="252" t="s">
@@ -15015,10 +15125,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="60">
-      <c r="A24" s="443" t="s">
+      <c r="A24" s="261" t="s">
         <v>974</v>
       </c>
-      <c r="B24" s="459" t="s">
+      <c r="B24" s="277" t="s">
         <v>981</v>
       </c>
       <c r="C24" s="252" t="s">
@@ -15026,10 +15136,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="75">
-      <c r="A25" s="443" t="s">
+      <c r="A25" s="261" t="s">
         <v>975</v>
       </c>
-      <c r="B25" s="449" t="s">
+      <c r="B25" s="267" t="s">
         <v>941</v>
       </c>
       <c r="C25" s="252" t="s">
@@ -15037,10 +15147,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="90">
-      <c r="A26" s="443" t="s">
+      <c r="A26" s="261" t="s">
         <v>976</v>
       </c>
-      <c r="B26" s="460" t="s">
+      <c r="B26" s="278" t="s">
         <v>984</v>
       </c>
       <c r="C26" s="252" t="s">
@@ -15048,10 +15158,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="60">
-      <c r="A27" s="443" t="s">
+      <c r="A27" s="261" t="s">
         <v>977</v>
       </c>
-      <c r="B27" s="461" t="s">
+      <c r="B27" s="279" t="s">
         <v>744</v>
       </c>
       <c r="C27" s="252" t="s">
@@ -15059,10 +15169,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="60">
-      <c r="A28" s="443" t="s">
+      <c r="A28" s="261" t="s">
         <v>987</v>
       </c>
-      <c r="B28" s="446" t="s">
+      <c r="B28" s="264" t="s">
         <v>934</v>
       </c>
       <c r="C28" s="252" t="s">
@@ -15070,10 +15180,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="60">
-      <c r="A29" s="443" t="s">
+      <c r="A29" s="261" t="s">
         <v>988</v>
       </c>
-      <c r="B29" s="460" t="s">
+      <c r="B29" s="278" t="s">
         <v>984</v>
       </c>
       <c r="C29" s="252" t="s">
@@ -15081,10 +15191,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="60">
-      <c r="A30" s="443" t="s">
+      <c r="A30" s="261" t="s">
         <v>989</v>
       </c>
-      <c r="B30" s="444" t="s">
+      <c r="B30" s="262" t="s">
         <v>931</v>
       </c>
       <c r="C30" s="252" t="s">
@@ -15092,10 +15202,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="75">
-      <c r="A31" s="443" t="s">
+      <c r="A31" s="261" t="s">
         <v>990</v>
       </c>
-      <c r="B31" s="437" t="s">
+      <c r="B31" s="255" t="s">
         <v>929</v>
       </c>
       <c r="C31" s="252" t="s">
@@ -15103,10 +15213,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="255">
-      <c r="A32" s="443" t="s">
+      <c r="A32" s="261" t="s">
         <v>991</v>
       </c>
-      <c r="B32" s="449" t="s">
+      <c r="B32" s="267" t="s">
         <v>941</v>
       </c>
       <c r="C32" s="252" t="s">
@@ -15114,10 +15224,10 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="75">
-      <c r="A33" s="443" t="s">
+      <c r="A33" s="261" t="s">
         <v>992</v>
       </c>
-      <c r="B33" s="455" t="s">
+      <c r="B33" s="273" t="s">
         <v>952</v>
       </c>
       <c r="C33" s="252" t="s">
@@ -15125,10 +15235,10 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="75">
-      <c r="A34" s="443" t="s">
+      <c r="A34" s="261" t="s">
         <v>993</v>
       </c>
-      <c r="B34" s="459" t="s">
+      <c r="B34" s="277" t="s">
         <v>981</v>
       </c>
       <c r="C34" s="252" t="s">
@@ -15136,10 +15246,10 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="60">
-      <c r="A35" s="443" t="s">
+      <c r="A35" s="261" t="s">
         <v>994</v>
       </c>
-      <c r="B35" s="450" t="s">
+      <c r="B35" s="268" t="s">
         <v>925</v>
       </c>
       <c r="C35" s="252" t="s">
@@ -15147,10 +15257,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="75">
-      <c r="A36" s="443" t="s">
+      <c r="A36" s="261" t="s">
         <v>995</v>
       </c>
-      <c r="B36" s="448" t="s">
+      <c r="B36" s="266" t="s">
         <v>937</v>
       </c>
       <c r="C36" s="252" t="s">
@@ -15197,8 +15307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="11.25"/>
@@ -15214,28 +15324,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="12" thickBot="1">
-      <c r="B1" s="358" t="s">
+      <c r="B1" s="391" t="s">
         <v>504</v>
       </c>
-      <c r="C1" s="358"/>
-      <c r="D1" s="358"/>
-      <c r="E1" s="359"/>
-      <c r="F1" s="359"/>
-      <c r="G1" s="359"/>
-      <c r="H1" s="359"/>
-      <c r="I1" s="359"/>
+      <c r="C1" s="391"/>
+      <c r="D1" s="391"/>
+      <c r="E1" s="392"/>
+      <c r="F1" s="392"/>
+      <c r="G1" s="392"/>
+      <c r="H1" s="392"/>
+      <c r="I1" s="392"/>
     </row>
     <row r="2" spans="2:9" ht="12" thickBot="1">
       <c r="B2" s="131"/>
       <c r="C2" s="131"/>
       <c r="D2" s="131"/>
-      <c r="E2" s="355" t="s">
+      <c r="E2" s="388" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="356"/>
-      <c r="G2" s="356"/>
-      <c r="H2" s="356"/>
-      <c r="I2" s="357"/>
+      <c r="F2" s="389"/>
+      <c r="G2" s="389"/>
+      <c r="H2" s="389"/>
+      <c r="I2" s="390"/>
     </row>
     <row r="3" spans="2:9" ht="12" thickBot="1">
       <c r="B3" s="131"/>
@@ -15300,7 +15410,7 @@
       <c r="I5" s="176"/>
     </row>
     <row r="6" spans="2:9" ht="78.75">
-      <c r="B6" s="352" t="s">
+      <c r="B6" s="385" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="139" t="s">
@@ -15326,7 +15436,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="90">
-      <c r="B7" s="353"/>
+      <c r="B7" s="386"/>
       <c r="C7" s="140" t="s">
         <v>149</v>
       </c>
@@ -15350,7 +15460,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="56.25">
-      <c r="B8" s="353"/>
+      <c r="B8" s="386"/>
       <c r="C8" s="140" t="s">
         <v>72</v>
       </c>
@@ -15374,7 +15484,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="101.25">
-      <c r="B9" s="353"/>
+      <c r="B9" s="386"/>
       <c r="C9" s="140" t="s">
         <v>73</v>
       </c>
@@ -15398,7 +15508,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="67.5">
-      <c r="B10" s="353"/>
+      <c r="B10" s="386"/>
       <c r="C10" s="140" t="s">
         <v>99</v>
       </c>
@@ -15422,7 +15532,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="68.25" thickBot="1">
-      <c r="B11" s="353"/>
+      <c r="B11" s="386"/>
       <c r="C11" s="140" t="s">
         <v>74</v>
       </c>
@@ -15445,8 +15555,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="112.5">
-      <c r="B12" s="352" t="s">
+    <row r="12" spans="2:9" ht="101.25">
+      <c r="B12" s="385" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="141" t="s">
@@ -15472,7 +15582,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="101.25">
-      <c r="B13" s="353"/>
+      <c r="B13" s="386"/>
       <c r="C13" s="141" t="s">
         <v>77</v>
       </c>
@@ -15496,7 +15606,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="101.25">
-      <c r="B14" s="353"/>
+      <c r="B14" s="386"/>
       <c r="C14" s="141" t="s">
         <v>78</v>
       </c>
@@ -15520,7 +15630,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="102" thickBot="1">
-      <c r="B15" s="354"/>
+      <c r="B15" s="387"/>
       <c r="C15" s="141" t="s">
         <v>98</v>
       </c>
@@ -15544,7 +15654,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" ht="90">
-      <c r="B16" s="352" t="s">
+      <c r="B16" s="385" t="s">
         <v>76</v>
       </c>
       <c r="C16" s="141" t="s">
@@ -15570,7 +15680,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="101.25">
-      <c r="B17" s="353"/>
+      <c r="B17" s="386"/>
       <c r="C17" s="141" t="s">
         <v>80</v>
       </c>
@@ -15594,7 +15704,7 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="56.25">
-      <c r="B18" s="353"/>
+      <c r="B18" s="386"/>
       <c r="C18" s="141" t="s">
         <v>124</v>
       </c>
@@ -15618,7 +15728,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="113.25" thickBot="1">
-      <c r="B19" s="354"/>
+      <c r="B19" s="387"/>
       <c r="C19" s="141" t="s">
         <v>81</v>
       </c>
@@ -15642,7 +15752,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" ht="90">
-      <c r="B20" s="352" t="s">
+      <c r="B20" s="385" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="142" t="s">
@@ -15668,7 +15778,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="123.75">
-      <c r="B21" s="353"/>
+      <c r="B21" s="386"/>
       <c r="C21" s="142" t="s">
         <v>88</v>
       </c>
@@ -15692,7 +15802,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" ht="78.75">
-      <c r="B22" s="353"/>
+      <c r="B22" s="386"/>
       <c r="C22" s="142" t="s">
         <v>87</v>
       </c>
@@ -15716,7 +15826,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" ht="101.25">
-      <c r="B23" s="353"/>
+      <c r="B23" s="386"/>
       <c r="C23" s="142" t="s">
         <v>86</v>
       </c>
@@ -15739,8 +15849,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="112.5">
-      <c r="B24" s="353"/>
+    <row r="24" spans="2:9" ht="101.25">
+      <c r="B24" s="386"/>
       <c r="C24" s="142" t="s">
         <v>116</v>
       </c>
@@ -15764,7 +15874,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="56.25">
-      <c r="B25" s="353"/>
+      <c r="B25" s="386"/>
       <c r="C25" s="142" t="s">
         <v>85</v>
       </c>
@@ -15788,7 +15898,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="135">
-      <c r="B26" s="353"/>
+      <c r="B26" s="386"/>
       <c r="C26" s="142" t="s">
         <v>84</v>
       </c>
@@ -15812,7 +15922,7 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="135.75" thickBot="1">
-      <c r="B27" s="354"/>
+      <c r="B27" s="387"/>
       <c r="C27" s="143" t="s">
         <v>83</v>
       </c>
@@ -15856,8 +15966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B9"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -15866,28 +15976,28 @@
     <col min="3" max="3" width="40.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="7" max="7" width="55.7109375" customWidth="1"/>
+    <col min="8" max="8" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="46.5" customHeight="1" thickBot="1">
-      <c r="B2" s="360" t="s">
+      <c r="B2" s="393" t="s">
         <v>561</v>
       </c>
-      <c r="C2" s="360"/>
-      <c r="D2" s="360"/>
+      <c r="C2" s="393"/>
+      <c r="D2" s="393"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1">
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
-      <c r="D3" s="364" t="s">
+      <c r="D3" s="397" t="s">
         <v>425</v>
       </c>
-      <c r="E3" s="365"/>
-      <c r="F3" s="365"/>
-      <c r="G3" s="365"/>
-      <c r="H3" s="366"/>
+      <c r="E3" s="398"/>
+      <c r="F3" s="398"/>
+      <c r="G3" s="398"/>
+      <c r="H3" s="399"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1">
       <c r="B4" s="86"/>
@@ -15908,7 +16018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="24.75" thickBot="1">
+    <row r="5" spans="2:8" ht="15.75" thickBot="1">
       <c r="B5" s="107" t="s">
         <v>423</v>
       </c>
@@ -16031,8 +16141,8 @@
       <c r="G13" s="88"/>
       <c r="H13" s="89"/>
     </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="361" t="s">
+    <row r="14" spans="2:8" ht="48">
+      <c r="B14" s="394" t="s">
         <v>469</v>
       </c>
       <c r="C14" s="90" t="s">
@@ -16040,111 +16150,171 @@
       </c>
       <c r="D14" s="90"/>
       <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="91"/>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" s="362"/>
+      <c r="F14" s="90" t="s">
+        <v>1005</v>
+      </c>
+      <c r="G14" s="90" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H14" s="91" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="48">
+      <c r="B15" s="395"/>
       <c r="C15" s="92" t="s">
         <v>385</v>
       </c>
       <c r="D15" s="92"/>
       <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="93"/>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="B16" s="362"/>
+      <c r="F15" s="92" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G15" s="92" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H15" s="93" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="48">
+      <c r="B16" s="395"/>
       <c r="C16" s="92" t="s">
         <v>386</v>
       </c>
       <c r="D16" s="92"/>
       <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="93"/>
-    </row>
-    <row r="17" spans="2:8" ht="24">
-      <c r="B17" s="362"/>
+      <c r="F16" s="92" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G16" s="92" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H16" s="93" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="48">
+      <c r="B17" s="395"/>
       <c r="C17" s="92" t="s">
         <v>387</v>
       </c>
       <c r="D17" s="92"/>
       <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="93"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="362"/>
+      <c r="F17" s="92" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G17" s="92" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H17" s="93" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="36">
+      <c r="B18" s="395"/>
       <c r="C18" s="92" t="s">
         <v>388</v>
       </c>
       <c r="D18" s="92"/>
       <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="93"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="362"/>
+      <c r="F18" s="92" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G18" s="92" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H18" s="93" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="48">
+      <c r="B19" s="395"/>
       <c r="C19" s="92" t="s">
         <v>389</v>
       </c>
       <c r="D19" s="92"/>
       <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="93"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="362"/>
+      <c r="F19" s="92" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G19" s="92" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H19" s="93" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="48">
+      <c r="B20" s="395"/>
       <c r="C20" s="92" t="s">
         <v>390</v>
       </c>
       <c r="D20" s="92"/>
       <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="93"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="362"/>
-      <c r="C21" s="94" t="s">
+      <c r="F20" s="92" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G20" s="92" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H20" s="93" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="48">
+      <c r="B21" s="395"/>
+      <c r="C21" s="280" t="s">
         <v>391</v>
       </c>
       <c r="D21" s="94"/>
       <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="95"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="362"/>
-      <c r="C22" s="94" t="s">
+      <c r="F21" s="281" t="s">
+        <v>1027</v>
+      </c>
+      <c r="G21" s="281" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H21" s="282" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="48">
+      <c r="B22" s="395"/>
+      <c r="C22" s="281" t="s">
         <v>392</v>
       </c>
       <c r="D22" s="94"/>
       <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="95"/>
-    </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B23" s="363"/>
-      <c r="C23" s="96" t="s">
+      <c r="F22" s="281" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G22" s="281" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H22" s="282" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="48.75" thickBot="1">
+      <c r="B23" s="396"/>
+      <c r="C23" s="283" t="s">
         <v>393</v>
       </c>
       <c r="D23" s="96"/>
       <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="97"/>
+      <c r="F23" s="284" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G23" s="284" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H23" s="285" t="s">
+        <v>1034</v>
+      </c>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="361" t="s">
+      <c r="B24" s="394" t="s">
         <v>470</v>
       </c>
       <c r="C24" s="98" t="s">
@@ -16157,7 +16327,7 @@
       <c r="H24" s="99"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="362"/>
+      <c r="B25" s="395"/>
       <c r="C25" s="94" t="s">
         <v>395</v>
       </c>
@@ -16168,7 +16338,7 @@
       <c r="H25" s="95"/>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="362"/>
+      <c r="B26" s="395"/>
       <c r="C26" s="94" t="s">
         <v>396</v>
       </c>
@@ -16179,7 +16349,7 @@
       <c r="H26" s="95"/>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="362"/>
+      <c r="B27" s="395"/>
       <c r="C27" s="94" t="s">
         <v>397</v>
       </c>
@@ -16190,7 +16360,7 @@
       <c r="H27" s="95"/>
     </row>
     <row r="28" spans="2:8">
-      <c r="B28" s="362"/>
+      <c r="B28" s="395"/>
       <c r="C28" s="94" t="s">
         <v>398</v>
       </c>
@@ -16201,7 +16371,7 @@
       <c r="H28" s="95"/>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="362"/>
+      <c r="B29" s="395"/>
       <c r="C29" s="94" t="s">
         <v>399</v>
       </c>
@@ -16212,7 +16382,7 @@
       <c r="H29" s="95"/>
     </row>
     <row r="30" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B30" s="363"/>
+      <c r="B30" s="396"/>
       <c r="C30" s="96" t="s">
         <v>400</v>
       </c>
@@ -16223,7 +16393,7 @@
       <c r="H30" s="97"/>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="361" t="s">
+      <c r="B31" s="394" t="s">
         <v>471</v>
       </c>
       <c r="C31" s="98" t="s">
@@ -16236,7 +16406,7 @@
       <c r="H31" s="99"/>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="362"/>
+      <c r="B32" s="395"/>
       <c r="C32" s="94" t="s">
         <v>402</v>
       </c>
@@ -16247,7 +16417,7 @@
       <c r="H32" s="95"/>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="362"/>
+      <c r="B33" s="395"/>
       <c r="C33" s="94" t="s">
         <v>403</v>
       </c>
@@ -16258,7 +16428,7 @@
       <c r="H33" s="95"/>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="362"/>
+      <c r="B34" s="395"/>
       <c r="C34" s="94" t="s">
         <v>404</v>
       </c>
@@ -16269,7 +16439,7 @@
       <c r="H34" s="95"/>
     </row>
     <row r="35" spans="2:8">
-      <c r="B35" s="362"/>
+      <c r="B35" s="395"/>
       <c r="C35" s="94" t="s">
         <v>405</v>
       </c>
@@ -16280,7 +16450,7 @@
       <c r="H35" s="95"/>
     </row>
     <row r="36" spans="2:8">
-      <c r="B36" s="362"/>
+      <c r="B36" s="395"/>
       <c r="C36" s="94" t="s">
         <v>406</v>
       </c>
@@ -16291,7 +16461,7 @@
       <c r="H36" s="95"/>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="362"/>
+      <c r="B37" s="395"/>
       <c r="C37" s="94" t="s">
         <v>407</v>
       </c>
@@ -16302,7 +16472,7 @@
       <c r="H37" s="95"/>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="362"/>
+      <c r="B38" s="395"/>
       <c r="C38" s="94" t="s">
         <v>408</v>
       </c>
@@ -16313,7 +16483,7 @@
       <c r="H38" s="95"/>
     </row>
     <row r="39" spans="2:8">
-      <c r="B39" s="362"/>
+      <c r="B39" s="395"/>
       <c r="C39" s="94" t="s">
         <v>409</v>
       </c>
@@ -16324,7 +16494,7 @@
       <c r="H39" s="95"/>
     </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="362"/>
+      <c r="B40" s="395"/>
       <c r="C40" s="94" t="s">
         <v>410</v>
       </c>
@@ -16335,7 +16505,7 @@
       <c r="H40" s="95"/>
     </row>
     <row r="41" spans="2:8">
-      <c r="B41" s="362"/>
+      <c r="B41" s="395"/>
       <c r="C41" s="94" t="s">
         <v>411</v>
       </c>
@@ -16346,7 +16516,7 @@
       <c r="H41" s="95"/>
     </row>
     <row r="42" spans="2:8">
-      <c r="B42" s="362"/>
+      <c r="B42" s="395"/>
       <c r="C42" s="94" t="s">
         <v>412</v>
       </c>
@@ -16357,7 +16527,7 @@
       <c r="H42" s="95"/>
     </row>
     <row r="43" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B43" s="363"/>
+      <c r="B43" s="396"/>
       <c r="C43" s="96" t="s">
         <v>413</v>
       </c>
@@ -16368,7 +16538,7 @@
       <c r="H43" s="97"/>
     </row>
     <row r="44" spans="2:8">
-      <c r="B44" s="361" t="s">
+      <c r="B44" s="394" t="s">
         <v>472</v>
       </c>
       <c r="C44" s="98" t="s">
@@ -16381,7 +16551,7 @@
       <c r="H44" s="99"/>
     </row>
     <row r="45" spans="2:8">
-      <c r="B45" s="362"/>
+      <c r="B45" s="395"/>
       <c r="C45" s="94" t="s">
         <v>415</v>
       </c>
@@ -16392,7 +16562,7 @@
       <c r="H45" s="95"/>
     </row>
     <row r="46" spans="2:8">
-      <c r="B46" s="362"/>
+      <c r="B46" s="395"/>
       <c r="C46" s="94" t="s">
         <v>416</v>
       </c>
@@ -16403,7 +16573,7 @@
       <c r="H46" s="95"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B47" s="363"/>
+      <c r="B47" s="396"/>
       <c r="C47" s="96" t="s">
         <v>417</v>
       </c>
@@ -16444,20 +16614,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="46.5" customHeight="1" thickBot="1">
-      <c r="B2" s="370" t="s">
+      <c r="B2" s="403" t="s">
         <v>636</v>
       </c>
-      <c r="C2" s="370"/>
-      <c r="D2" s="370"/>
-      <c r="E2" s="370"/>
+      <c r="C2" s="403"/>
+      <c r="D2" s="403"/>
+      <c r="E2" s="403"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B3" s="367" t="s">
+      <c r="B3" s="400" t="s">
         <v>607</v>
       </c>
-      <c r="C3" s="368"/>
-      <c r="D3" s="368"/>
-      <c r="E3" s="369"/>
+      <c r="C3" s="401"/>
+      <c r="D3" s="401"/>
+      <c r="E3" s="402"/>
     </row>
     <row r="4" spans="2:5" ht="24.75" thickBot="1">
       <c r="B4" s="107" t="s">
@@ -16540,12 +16710,12 @@
       <c r="E10" s="198"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B11" s="367" t="s">
+      <c r="B11" s="400" t="s">
         <v>607</v>
       </c>
-      <c r="C11" s="368"/>
-      <c r="D11" s="368"/>
-      <c r="E11" s="369"/>
+      <c r="C11" s="401"/>
+      <c r="D11" s="401"/>
+      <c r="E11" s="402"/>
     </row>
     <row r="12" spans="2:5" ht="24.75" thickBot="1">
       <c r="B12" s="107" t="s">
@@ -16572,7 +16742,7 @@
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="361" t="s">
+      <c r="B14" s="394" t="s">
         <v>475</v>
       </c>
       <c r="C14" s="90" t="s">
@@ -16582,7 +16752,7 @@
       <c r="E14" s="91"/>
     </row>
     <row r="15" spans="2:5" ht="36">
-      <c r="B15" s="362"/>
+      <c r="B15" s="395"/>
       <c r="C15" s="92" t="s">
         <v>610</v>
       </c>
@@ -16590,7 +16760,7 @@
       <c r="E15" s="93"/>
     </row>
     <row r="16" spans="2:5" ht="24.75" thickBot="1">
-      <c r="B16" s="363"/>
+      <c r="B16" s="396"/>
       <c r="C16" s="199" t="s">
         <v>611</v>
       </c>
@@ -16598,7 +16768,7 @@
       <c r="E16" s="150"/>
     </row>
     <row r="17" spans="2:5" ht="24">
-      <c r="B17" s="361" t="s">
+      <c r="B17" s="394" t="s">
         <v>489</v>
       </c>
       <c r="C17" s="90" t="s">
@@ -16608,7 +16778,7 @@
       <c r="E17" s="193"/>
     </row>
     <row r="18" spans="2:5" ht="24">
-      <c r="B18" s="362"/>
+      <c r="B18" s="395"/>
       <c r="C18" s="92" t="s">
         <v>613</v>
       </c>
@@ -16616,7 +16786,7 @@
       <c r="E18" s="191"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="362"/>
+      <c r="B19" s="395"/>
       <c r="C19" s="92" t="s">
         <v>614</v>
       </c>
@@ -16624,7 +16794,7 @@
       <c r="E19" s="191"/>
     </row>
     <row r="20" spans="2:5" ht="24">
-      <c r="B20" s="362"/>
+      <c r="B20" s="395"/>
       <c r="C20" s="92" t="s">
         <v>615</v>
       </c>
@@ -16632,7 +16802,7 @@
       <c r="E20" s="194"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B21" s="363"/>
+      <c r="B21" s="396"/>
       <c r="C21" s="199" t="s">
         <v>622</v>
       </c>
@@ -16640,7 +16810,7 @@
       <c r="E21" s="150"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="361" t="s">
+      <c r="B22" s="394" t="s">
         <v>495</v>
       </c>
       <c r="C22" s="90" t="s">
@@ -16650,7 +16820,7 @@
       <c r="E22" s="193"/>
     </row>
     <row r="23" spans="2:5" ht="36">
-      <c r="B23" s="362"/>
+      <c r="B23" s="395"/>
       <c r="C23" s="92" t="s">
         <v>617</v>
       </c>
@@ -16658,7 +16828,7 @@
       <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="362"/>
+      <c r="B24" s="395"/>
       <c r="C24" s="92" t="s">
         <v>618</v>
       </c>
@@ -16666,7 +16836,7 @@
       <c r="E24" s="191"/>
     </row>
     <row r="25" spans="2:5" ht="24.75" thickBot="1">
-      <c r="B25" s="363"/>
+      <c r="B25" s="396"/>
       <c r="C25" s="199" t="s">
         <v>619</v>
       </c>
@@ -16674,7 +16844,7 @@
       <c r="E25" s="150"/>
     </row>
     <row r="26" spans="2:5" ht="36">
-      <c r="B26" s="361" t="s">
+      <c r="B26" s="394" t="s">
         <v>476</v>
       </c>
       <c r="C26" s="90" t="s">
@@ -16684,7 +16854,7 @@
       <c r="E26" s="193"/>
     </row>
     <row r="27" spans="2:5" ht="24">
-      <c r="B27" s="362"/>
+      <c r="B27" s="395"/>
       <c r="C27" s="92" t="s">
         <v>620</v>
       </c>
@@ -16692,7 +16862,7 @@
       <c r="E27" s="191"/>
     </row>
     <row r="28" spans="2:5" ht="24.75" thickBot="1">
-      <c r="B28" s="363"/>
+      <c r="B28" s="396"/>
       <c r="C28" s="199" t="s">
         <v>621</v>
       </c>

</xml_diff>